<commit_message>
[DEV] Center FE pin worths
Output files provided for special center fuel element pin worths.
</commit_message>
<xml_diff>
--- a/snapReactors/reference_calc/DryExperiments.xlsx
+++ b/snapReactors/reference_calc/DryExperiments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwprod-my.sharepoint.com/personal/sgarcia9_wisc_edu/Documents/GradSchool Homework/Misc. Research/DiffDrumWorth/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwprod.sharepoint.com/sites/ReTI/Shared Documents/SNAP/Dry Experiments Calculations Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="939" documentId="8_{BEA5E111-021F-45DA-85BB-227D92BE1F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A3DFBA0-6B39-4D89-9521-12D8A1A7A952}"/>
+  <xr:revisionPtr revIDLastSave="1019" documentId="8_{BEA5E111-021F-45DA-85BB-227D92BE1F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76A59CCE-5A80-4176-BE1A-7D1B46CF3BE7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{69F113DC-7633-4730-BD7E-3337CEB2EA1E}"/>
+    <workbookView xWindow="-28920" yWindow="2565" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{69F113DC-7633-4730-BD7E-3337CEB2EA1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Differential &amp; Integral" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="84">
   <si>
     <t>A Shim Rotation</t>
   </si>
@@ -169,25 +169,43 @@
     <t>Void I-1</t>
   </si>
   <si>
+    <t>Needs to be redone with air // done</t>
+  </si>
+  <si>
     <t>E-672</t>
   </si>
   <si>
     <t>E-181 I-1</t>
   </si>
   <si>
+    <t>Needs to be redone with proper fuel // done</t>
+  </si>
+  <si>
     <t>E-669</t>
+  </si>
+  <si>
+    <t>E-672 I-1</t>
   </si>
   <si>
     <t>E-671</t>
   </si>
   <si>
+    <t>E-669 I-1</t>
+  </si>
+  <si>
     <t>E-661</t>
+  </si>
+  <si>
+    <t>E-671 I-1</t>
   </si>
   <si>
     <t>E-660</t>
   </si>
   <si>
     <t>V-23</t>
+  </si>
+  <si>
+    <t>E-661 I-1</t>
   </si>
   <si>
     <t>IX-45</t>
@@ -487,7 +505,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -527,17 +545,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6480,7 +6501,7 @@
   <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8333,10 +8354,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A0E277-164D-40AC-8934-6E7AB0E9B78A}">
-  <dimension ref="A1:R49"/>
+  <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8349,53 +8370,56 @@
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:21">
+      <c r="A1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="25" t="s">
+      <c r="G1" s="23"/>
+      <c r="H1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="M1" s="23" t="s">
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="M1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
     </row>
-    <row r="2" spans="1:18">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+    <row r="2" spans="1:21">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="F2" s="18" t="s">
         <v>24</v>
       </c>
@@ -8433,7 +8457,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:21">
       <c r="A3" s="15" t="s">
         <v>33</v>
       </c>
@@ -8461,8 +8485,8 @@
         <v>0</v>
       </c>
       <c r="I3" s="15">
-        <f>(R3-R4)</f>
-        <v>53.194652857019548</v>
+        <f>ABS(R3-$R$4)</f>
+        <v>59.014840034822171</v>
       </c>
       <c r="J3" s="15">
         <f>ABS(H3-F3)</f>
@@ -8470,28 +8494,31 @@
       </c>
       <c r="K3" s="15">
         <f>ABS(I3-G3)</f>
-        <v>8.1946528570195483</v>
+        <v>14.014840034822171</v>
       </c>
       <c r="M3" t="s">
         <v>36</v>
       </c>
       <c r="N3" s="8">
-        <v>0.99750300000000003</v>
-      </c>
-      <c r="O3">
-        <v>-2.5032506167900963E-3</v>
+        <v>0.99803699999999995</v>
+      </c>
+      <c r="O3" s="8">
+        <f>(N3-1)/N3</f>
+        <v>-1.9668609480410527E-3</v>
       </c>
       <c r="P3" s="8">
-        <v>7.9136299999999996E-3</v>
-      </c>
-      <c r="Q3">
-        <v>-0.3163214121446285</v>
-      </c>
-      <c r="R3">
-        <v>-31.632141214462848</v>
+        <v>7.8902099999999999E-3</v>
+      </c>
+      <c r="Q3" s="8">
+        <f>O3/P3</f>
+        <v>-0.2492786564668181</v>
+      </c>
+      <c r="R3" s="8">
+        <f>Q3*100</f>
+        <v>-24.927865646681809</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:21">
       <c r="A4" s="15" t="s">
         <v>37</v>
       </c>
@@ -8515,42 +8542,50 @@
       </c>
       <c r="H4" s="15">
         <f>ABS(R5-R3)</f>
-        <v>4.5900704347669823</v>
+        <v>0.96338255778946191</v>
       </c>
       <c r="I4" s="15">
-        <f>R5-R4</f>
-        <v>57.784723291786534</v>
+        <f>ABS(R5-$R$4)</f>
+        <v>59.97822259261163</v>
       </c>
       <c r="J4" s="15">
         <f>ABS(H4-F4)</f>
-        <v>3.1900704347669824</v>
+        <v>0.436617442210538</v>
       </c>
       <c r="K4" s="15">
         <f>ABS(I4-G4)</f>
-        <v>11.384723291786536</v>
+        <v>13.578222592611631</v>
       </c>
       <c r="M4" t="s">
         <v>38</v>
       </c>
       <c r="N4" s="8">
-        <v>0.99332799999999999</v>
-      </c>
-      <c r="O4">
-        <v>-6.7168145869239684E-3</v>
+        <v>0.99340600000000001</v>
+      </c>
+      <c r="O4" s="8">
+        <f>(N4-1)/N4</f>
+        <v>-6.6377694517649266E-3</v>
       </c>
       <c r="P4" s="8">
-        <v>7.9182699999999998E-3</v>
-      </c>
-      <c r="Q4">
-        <v>-0.84826794071482392</v>
-      </c>
-      <c r="R4">
-        <v>-84.826794071482396</v>
-      </c>
+        <v>7.9074999999999996E-3</v>
+      </c>
+      <c r="Q4" s="8">
+        <f>O4/P4</f>
+        <v>-0.83942705681503982</v>
+      </c>
+      <c r="R4" s="8">
+        <f>Q4*100</f>
+        <v>-83.94270568150398</v>
+      </c>
+      <c r="S4" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:21">
       <c r="A5" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B5" s="16">
         <v>311.5</v>
@@ -8570,35 +8605,52 @@
       <c r="G5" s="15">
         <v>49.3</v>
       </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
+      <c r="H5" s="15">
+        <f>ABS(R6-R3)</f>
+        <v>4.9356544432315772</v>
+      </c>
+      <c r="I5" s="15">
+        <f t="shared" ref="I5:I8" si="0">ABS(R6-$R$4)</f>
+        <v>63.950494478053749</v>
+      </c>
+      <c r="J5" s="15">
+        <f t="shared" ref="J5:J8" si="1">ABS(H5-F5)</f>
+        <v>0.63565444323157738</v>
+      </c>
+      <c r="K5" s="15">
+        <f t="shared" ref="K5:K8" si="2">ABS(I5-G5)</f>
+        <v>14.650494478053751</v>
+      </c>
       <c r="M5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N5" s="8">
-        <v>0.99786699999999995</v>
+        <v>0.99810600000000005</v>
       </c>
       <c r="O5" s="8">
         <f>(N5-1)/N5</f>
-        <v>-2.1375594142306054E-3</v>
+        <v>-1.8975940431176159E-3</v>
       </c>
       <c r="P5" s="9">
-        <v>7.9045699999999997E-3</v>
+        <v>7.9183599999999993E-3</v>
       </c>
       <c r="Q5" s="8">
         <f>O5/P5</f>
-        <v>-0.27042070779695865</v>
+        <v>-0.23964483088892347</v>
       </c>
       <c r="R5">
         <f>Q5*100</f>
-        <v>-27.042070779695866</v>
-      </c>
+        <v>-23.964483088892347</v>
+      </c>
+      <c r="S5" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="T5" s="25"/>
+      <c r="U5" s="25"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:21">
       <c r="A6" s="15" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B6" s="15">
         <v>317.3</v>
@@ -8618,14 +8670,47 @@
       <c r="G6" s="15">
         <v>50.8</v>
       </c>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
+      <c r="H6" s="15">
+        <f>ABS(R7-R3)</f>
+        <v>2.5841262237683651</v>
+      </c>
+      <c r="I6" s="15">
+        <f t="shared" si="0"/>
+        <v>61.598966258590536</v>
+      </c>
+      <c r="J6" s="15">
+        <f t="shared" si="1"/>
+        <v>3.2158737762316347</v>
+      </c>
+      <c r="K6" s="15">
+        <f t="shared" si="2"/>
+        <v>10.798966258590539</v>
+      </c>
+      <c r="M6" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" s="8">
+        <v>0.99841800000000003</v>
+      </c>
+      <c r="O6" s="8">
+        <f t="shared" ref="O6:O10" si="3">(N6-1)/N6</f>
+        <v>-1.5845066895828924E-3</v>
+      </c>
+      <c r="P6" s="8">
+        <v>7.9256199999999995E-3</v>
+      </c>
+      <c r="Q6" s="8">
+        <f t="shared" ref="Q6:Q9" si="4">O6/P6</f>
+        <v>-0.19992211203450233</v>
+      </c>
+      <c r="R6">
+        <f t="shared" ref="R6:R9" si="5">Q6*100</f>
+        <v>-19.992211203450232</v>
+      </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:21">
       <c r="A7" s="15" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B7" s="15">
         <v>293.89999999999998</v>
@@ -8645,14 +8730,47 @@
       <c r="G7" s="15">
         <v>48.5</v>
       </c>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
+      <c r="H7" s="15">
+        <f>ABS(R8-R3)</f>
+        <v>5.4432386095736689</v>
+      </c>
+      <c r="I7" s="15">
+        <f t="shared" si="0"/>
+        <v>53.571601425248502</v>
+      </c>
+      <c r="J7" s="15">
+        <f t="shared" si="1"/>
+        <v>1.9432386095736689</v>
+      </c>
+      <c r="K7" s="15">
+        <f t="shared" si="2"/>
+        <v>5.0716014252485024</v>
+      </c>
+      <c r="M7" t="s">
+        <v>46</v>
+      </c>
+      <c r="N7" s="8">
+        <v>0.99823600000000001</v>
+      </c>
+      <c r="O7" s="8">
+        <f t="shared" si="3"/>
+        <v>-1.7671171947314941E-3</v>
+      </c>
+      <c r="P7" s="8">
+        <v>7.9087800000000007E-3</v>
+      </c>
+      <c r="Q7" s="8">
+        <f t="shared" si="4"/>
+        <v>-0.22343739422913445</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="5"/>
+        <v>-22.343739422913444</v>
+      </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:21">
       <c r="A8" s="15" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B8" s="15">
         <v>278</v>
@@ -8672,14 +8790,47 @@
       <c r="G8" s="15">
         <v>11.5</v>
       </c>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
+      <c r="H8" s="15">
+        <f>ABS(R9-R3)</f>
+        <v>47.45052758724519</v>
+      </c>
+      <c r="I8" s="15">
+        <f t="shared" si="0"/>
+        <v>11.564312447576981</v>
+      </c>
+      <c r="J8" s="15">
+        <f t="shared" si="1"/>
+        <v>47.45052758724519</v>
+      </c>
+      <c r="K8" s="15">
+        <f t="shared" si="2"/>
+        <v>6.4312447576980958E-2</v>
+      </c>
+      <c r="M8" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" s="8">
+        <v>0.99760700000000002</v>
+      </c>
+      <c r="O8" s="8">
+        <f t="shared" si="3"/>
+        <v>-2.3987401852633137E-3</v>
+      </c>
+      <c r="P8" s="8">
+        <v>7.8980999999999999E-3</v>
+      </c>
+      <c r="Q8" s="8">
+        <f t="shared" si="4"/>
+        <v>-0.30371104256255477</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="5"/>
+        <v>-30.371104256255478</v>
+      </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:21">
       <c r="A9" s="15" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B9" s="15">
         <v>278.3</v>
@@ -8691,7 +8842,7 @@
         <v>9.7799999999999994</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F9" s="15">
         <v>0</v>
@@ -8703,10 +8854,31 @@
       <c r="I9" s="15"/>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
+      <c r="M9" t="s">
+        <v>51</v>
+      </c>
+      <c r="N9" s="8">
+        <v>0.99429400000000001</v>
+      </c>
+      <c r="O9" s="8">
+        <f t="shared" si="3"/>
+        <v>-5.7387452805709267E-3</v>
+      </c>
+      <c r="P9" s="8">
+        <v>7.9288099999999997E-3</v>
+      </c>
+      <c r="Q9" s="8">
+        <f t="shared" si="4"/>
+        <v>-0.72378393233926996</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="5"/>
+        <v>-72.378393233927</v>
+      </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:21">
       <c r="A10" s="15" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B10" s="15">
         <v>278</v>
@@ -8718,7 +8890,7 @@
         <v>9.5399999999999991</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F10" s="15">
         <v>0</v>
@@ -8730,10 +8902,11 @@
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
+      <c r="O10" s="8"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:21">
       <c r="A11" s="15" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B11" s="15">
         <v>278</v>
@@ -8745,7 +8918,7 @@
         <v>9.5399999999999991</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="F11" s="15">
         <v>0</v>
@@ -8760,42 +8933,42 @@
     </row>
     <row r="22" spans="1:11">
       <c r="F22" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="D24" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="24" t="s">
+      <c r="E24" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F24" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="G24" s="24"/>
-      <c r="H24" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
+      <c r="F24" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="23"/>
+      <c r="H24" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
       <c r="F25" s="18" t="s">
         <v>24</v>
       </c>
@@ -8809,10 +8982,10 @@
         <v>25</v>
       </c>
       <c r="J25" s="19" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="K25" s="19" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -8842,9 +9015,9 @@
         <f>ABS(R16-R16)</f>
         <v>0</v>
       </c>
-      <c r="I26" s="15">
+      <c r="I26" s="16">
         <f>(O3-O4)*10^5</f>
-        <v>421.35639701338727</v>
+        <v>467.09085037238737</v>
       </c>
       <c r="J26" s="15">
         <f>ABS(H26-F26)</f>
@@ -8852,7 +9025,7 @@
       </c>
       <c r="K26" s="15">
         <f>ABS(I26-G26)</f>
-        <v>74.856397013387266</v>
+        <v>120.59085037238737</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -8879,26 +9052,26 @@
         <f>G4/100*0.0077*10^5</f>
         <v>357.28</v>
       </c>
-      <c r="H27" s="15">
-        <f>ABS(O5-O3)*10^5</f>
-        <v>36.569120255949088</v>
+      <c r="H27" s="16">
+        <f>ABS(O5-$O$3)*10^5</f>
+        <v>6.9266904923436865</v>
       </c>
       <c r="I27" s="16">
-        <f>(O5-O4)*10^5</f>
-        <v>457.9255172693363</v>
+        <f>(O5-$O$4)*10^5</f>
+        <v>474.01754086473107</v>
       </c>
       <c r="J27" s="15">
         <f>ABS(H27-F27)</f>
-        <v>25.789120255949086</v>
+        <v>3.8533095076563129</v>
       </c>
       <c r="K27" s="15">
         <f>ABS(I27-G27)</f>
-        <v>100.64551726933632</v>
+        <v>116.7375408647311</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B28" s="16">
         <v>311.5</v>
@@ -8913,21 +9086,33 @@
         <v>35</v>
       </c>
       <c r="F28" s="15">
-        <f t="shared" ref="F28:G34" si="0">F5/100*0.0077*10^5</f>
+        <f t="shared" ref="F28:G34" si="6">F5/100*0.0077*10^5</f>
         <v>33.11</v>
       </c>
       <c r="G28" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>379.61</v>
       </c>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
+      <c r="H28" s="16">
+        <f t="shared" ref="H28:H34" si="7">ABS(O6-$O$3)*10^5</f>
+        <v>38.235425845816039</v>
+      </c>
+      <c r="I28" s="16">
+        <f t="shared" ref="I28:I34" si="8">(O6-$O$4)*10^5</f>
+        <v>505.32627621820336</v>
+      </c>
+      <c r="J28" s="15">
+        <f t="shared" ref="J28:J34" si="9">ABS(H28-F28)</f>
+        <v>5.1254258458160393</v>
+      </c>
+      <c r="K28" s="15">
+        <f t="shared" ref="K28:K34" si="10">ABS(I28-G28)</f>
+        <v>125.71627621820335</v>
+      </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="15" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B29" s="15">
         <v>317.3</v>
@@ -8942,21 +9127,33 @@
         <v>35</v>
       </c>
       <c r="F29" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>44.66</v>
       </c>
       <c r="G29" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>391.16</v>
       </c>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
+      <c r="H29" s="16">
+        <f t="shared" si="7"/>
+        <v>19.974375330955866</v>
+      </c>
+      <c r="I29" s="16">
+        <f t="shared" si="8"/>
+        <v>487.06522570334323</v>
+      </c>
+      <c r="J29" s="15">
+        <f t="shared" si="9"/>
+        <v>24.685624669044131</v>
+      </c>
+      <c r="K29" s="15">
+        <f t="shared" si="10"/>
+        <v>95.905225703343206</v>
+      </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="15" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B30" s="15">
         <v>293.89999999999998</v>
@@ -8971,21 +9168,33 @@
         <v>35</v>
       </c>
       <c r="F30" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>26.950000000000003</v>
       </c>
       <c r="G30" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>373.45</v>
       </c>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
+      <c r="H30" s="16">
+        <f t="shared" si="7"/>
+        <v>43.187923722226095</v>
+      </c>
+      <c r="I30" s="16">
+        <f t="shared" si="8"/>
+        <v>423.90292665016125</v>
+      </c>
+      <c r="J30" s="15">
+        <f t="shared" si="9"/>
+        <v>16.237923722226093</v>
+      </c>
+      <c r="K30" s="15">
+        <f t="shared" si="10"/>
+        <v>50.45292665016126</v>
+      </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="15" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B31" s="15">
         <v>278</v>
@@ -9000,21 +9209,30 @@
         <v>35</v>
       </c>
       <c r="F31" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G31" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>88.550000000000011</v>
       </c>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
+      <c r="H31" s="16">
+        <f t="shared" si="7"/>
+        <v>377.18843325298741</v>
+      </c>
+      <c r="I31" s="16">
+        <f t="shared" si="8"/>
+        <v>89.902417119399999</v>
+      </c>
       <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
+      <c r="K31" s="15">
+        <f t="shared" si="10"/>
+        <v>1.3524171193999877</v>
+      </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="15" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B32" s="15">
         <v>278.3</v>
@@ -9026,24 +9244,33 @@
         <v>9.7799999999999994</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F32" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G32" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>69.3</v>
       </c>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
+      <c r="H32" s="16">
+        <f t="shared" si="7"/>
+        <v>196.68609480410527</v>
+      </c>
+      <c r="I32" s="16">
+        <f t="shared" si="8"/>
+        <v>663.77694517649263</v>
+      </c>
       <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
+      <c r="K32" s="15">
+        <f t="shared" si="10"/>
+        <v>594.47694517649268</v>
+      </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="15" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B33" s="15">
         <v>278</v>
@@ -9055,24 +9282,33 @@
         <v>9.5399999999999991</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F33" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G33" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>77</v>
       </c>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
+      <c r="H33" s="16">
+        <f t="shared" si="7"/>
+        <v>196.68609480410527</v>
+      </c>
+      <c r="I33" s="16">
+        <f t="shared" si="8"/>
+        <v>663.77694517649263</v>
+      </c>
       <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
+      <c r="K33" s="15">
+        <f t="shared" si="10"/>
+        <v>586.77694517649263</v>
+      </c>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="15" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B34" s="15">
         <v>278</v>
@@ -9084,55 +9320,64 @@
         <v>9.5399999999999991</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="F34" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G34" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>111.64999999999999</v>
       </c>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
+      <c r="H34" s="16">
+        <f t="shared" si="7"/>
+        <v>196.68609480410527</v>
+      </c>
+      <c r="I34" s="16">
+        <f t="shared" si="8"/>
+        <v>663.77694517649263</v>
+      </c>
       <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
+      <c r="K34" s="15">
+        <f t="shared" si="10"/>
+        <v>552.12694517649265</v>
+      </c>
     </row>
     <row r="39" spans="1:11">
-      <c r="A39" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="B39" s="23"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
+      <c r="A39" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D40" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="E40" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="F40" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="G40" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="I40" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="J40">
         <f>1E+24</f>
@@ -9141,7 +9386,7 @@
     </row>
     <row r="41" spans="1:11">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B41">
         <v>309.63</v>
@@ -9163,7 +9408,7 @@
         <v>6.06</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="J41" s="11">
         <v>2.54</v>
@@ -9183,21 +9428,21 @@
         <v>9.6999999999999993</v>
       </c>
       <c r="E42">
-        <f>E$41*$D42/$D$41</f>
+        <f t="shared" ref="E42:F49" si="11">E$41*$D42/$D$41</f>
         <v>1.0272912423625252E-4</v>
       </c>
       <c r="F42">
-        <f>F$41*$D42/$D$41</f>
+        <f t="shared" si="11"/>
         <v>1.4125254582484723E-3</v>
       </c>
       <c r="G42">
-        <f>B42/$J$47</f>
+        <f t="shared" ref="G42:G49" si="12">B42/$J$47</f>
         <v>6.0650947308232492</v>
       </c>
     </row>
     <row r="43" spans="1:11">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B43" s="8">
         <v>311.5</v>
@@ -9209,19 +9454,19 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="E43">
-        <f>E$41*$D43/$D$41</f>
+        <f t="shared" si="11"/>
         <v>1.0537678207739306E-4</v>
       </c>
       <c r="F43">
-        <f>F$41*$D43/$D$41</f>
+        <f t="shared" si="11"/>
         <v>1.4489307535641546E-3</v>
       </c>
       <c r="G43">
-        <f>B43/$J$47</f>
+        <f t="shared" si="12"/>
         <v>6.1082347515403885</v>
       </c>
       <c r="I43" s="11" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="J43" s="11">
         <f>0.532/2</f>
@@ -9230,7 +9475,7 @@
     </row>
     <row r="44" spans="1:11">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B44">
         <v>317.3</v>
@@ -9242,19 +9487,19 @@
         <v>10.11</v>
       </c>
       <c r="E44">
-        <f>E$41*$D44/$D$41</f>
+        <f t="shared" si="11"/>
         <v>1.0707128309572299E-4</v>
       </c>
       <c r="F44">
-        <f>F$41*$D44/$D$41</f>
+        <f t="shared" si="11"/>
         <v>1.4722301425661914E-3</v>
       </c>
       <c r="G44">
-        <f>B44/$J$47</f>
+        <f t="shared" si="12"/>
         <v>6.2219675334310285</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="J44" s="11">
         <v>14</v>
@@ -9262,7 +9507,7 @@
     </row>
     <row r="45" spans="1:11">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B45">
         <v>293.89999999999998</v>
@@ -9274,19 +9519,19 @@
         <v>9.32</v>
       </c>
       <c r="E45">
-        <f>E$41*$D45/$D$41</f>
+        <f t="shared" si="11"/>
         <v>9.8704684317718941E-5</v>
       </c>
       <c r="F45">
-        <f>F$41*$D45/$D$41</f>
+        <f t="shared" si="11"/>
         <v>1.3571894093686355E-3</v>
       </c>
       <c r="G45">
-        <f>B45/$J$47</f>
+        <f t="shared" si="12"/>
         <v>5.7631145858032751</v>
       </c>
       <c r="I45" s="11" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="J45" s="11">
         <f>J43*J41</f>
@@ -9295,7 +9540,7 @@
     </row>
     <row r="46" spans="1:11">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B46">
         <v>278</v>
@@ -9307,19 +9552,19 @@
         <v>9.5399999999999991</v>
       </c>
       <c r="E46">
-        <f>E$41*$D46/$D$41</f>
+        <f t="shared" si="11"/>
         <v>1.0103462321792258E-4</v>
       </c>
       <c r="F46">
-        <f>F$41*$D46/$D$41</f>
+        <f t="shared" si="11"/>
         <v>1.3892260692464358E-3</v>
       </c>
       <c r="G46">
-        <f>B46/$J$47</f>
+        <f t="shared" si="12"/>
         <v>5.4513298906203147</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="J46" s="11">
         <f>J44*J41</f>
@@ -9328,7 +9573,7 @@
     </row>
     <row r="47" spans="1:11">
       <c r="A47" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B47">
         <v>278.3</v>
@@ -9340,19 +9585,19 @@
         <v>9.7799999999999994</v>
       </c>
       <c r="E47">
-        <f>E$41*$D47/$D$41</f>
+        <f t="shared" si="11"/>
         <v>1.0357637474541749E-4</v>
       </c>
       <c r="F47">
-        <f>F$41*$D47/$D$41</f>
+        <f t="shared" si="11"/>
         <v>1.4241751527494908E-3</v>
       </c>
       <c r="G47">
-        <f>B47/$J$47</f>
+        <f t="shared" si="12"/>
         <v>5.4572126207181064</v>
       </c>
       <c r="I47" s="11" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="J47" s="11">
         <f>PI()*J45^2*J46</f>
@@ -9361,7 +9606,7 @@
     </row>
     <row r="48" spans="1:11">
       <c r="A48" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B48">
         <v>278</v>
@@ -9373,19 +9618,19 @@
         <v>9.5399999999999991</v>
       </c>
       <c r="E48">
-        <f>E$41*$D48/$D$41</f>
+        <f t="shared" si="11"/>
         <v>1.0103462321792258E-4</v>
       </c>
       <c r="F48">
-        <f>F$41*$D48/$D$41</f>
+        <f t="shared" si="11"/>
         <v>1.3892260692464358E-3</v>
       </c>
       <c r="G48">
-        <f>B48/$J$47</f>
+        <f t="shared" si="12"/>
         <v>5.4513298906203147</v>
       </c>
       <c r="I48" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="J48">
         <f>6.0221408E+23</f>
@@ -9394,7 +9639,7 @@
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B49">
         <v>278</v>
@@ -9406,27 +9651,26 @@
         <v>9.5399999999999991</v>
       </c>
       <c r="E49">
-        <f>E$41*$D49/$D$41</f>
+        <f t="shared" si="11"/>
         <v>1.0103462321792258E-4</v>
       </c>
       <c r="F49">
-        <f>F$41*$D49/$D$41</f>
+        <f t="shared" si="11"/>
         <v>1.3892260692464358E-3</v>
       </c>
       <c r="G49">
-        <f>B49/$J$47</f>
+        <f t="shared" si="12"/>
         <v>5.4513298906203147</v>
       </c>
       <c r="I49" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="J49">
         <v>6.06</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="M1:R1"/>
+  <mergeCells count="18">
     <mergeCell ref="A39:F39"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:K1"/>
@@ -9442,6 +9686,9 @@
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="M1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9468,24 +9715,24 @@
   <sheetData>
     <row r="2" spans="1:6">
       <c r="B2" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F2" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B3">
         <f>0.00797</f>
@@ -9504,7 +9751,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B4" s="9">
         <v>6.8426399999999998E-6</v>
@@ -9523,7 +9770,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B5">
         <f>B3/B4</f>
@@ -9559,17 +9806,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e1ecaa1f-5549-4843-8e0b-36d11b9c4a00" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02f07221-7782-4248-899f-09bd431cf93f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ABEDCDC6898E9D48B17B2D917023A0E9" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c9b35f98bcdb4a0d7929321150581d5e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="02f07221-7782-4248-899f-09bd431cf93f" xmlns:ns3="e1ecaa1f-5549-4843-8e0b-36d11b9c4a00" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="53fe39de12092328c3276185799bfa71" ns2:_="" ns3:_="">
     <xsd:import namespace="02f07221-7782-4248-899f-09bd431cf93f"/>
@@ -9806,6 +10042,24 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e1ecaa1f-5549-4843-8e0b-36d11b9c4a00" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02f07221-7782-4248-899f-09bd431cf93f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="e1ecaa1f-5549-4843-8e0b-36d11b9c4a00">
+      <UserInfo>
+        <DisplayName>Oliver Douglas Paleen</DisplayName>
+        <AccountId>61</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -9816,11 +10070,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A981A7-99F7-420B-92E3-468028514462}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4FEB34B-0950-495E-8A7D-7F2024A133DD}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4FEB34B-0950-495E-8A7D-7F2024A133DD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A981A7-99F7-420B-92E3-468028514462}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
[DEV] Fuel Element Experiment Materials update
Fuel composition definitions were updated to reflect changes to zirconium atomic densities changes, which were not previously captured. Adiditionally, excel file with calculations is updated as well.
</commit_message>
<xml_diff>
--- a/snapReactors/reference_calc/DryExperiments.xlsx
+++ b/snapReactors/reference_calc/DryExperiments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwprod.sharepoint.com/sites/ReTI/Shared Documents/SNAP/Dry Experiments Calculations Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1019" documentId="8_{BEA5E111-021F-45DA-85BB-227D92BE1F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76A59CCE-5A80-4176-BE1A-7D1B46CF3BE7}"/>
+  <xr:revisionPtr revIDLastSave="1196" documentId="8_{BEA5E111-021F-45DA-85BB-227D92BE1F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C35E55BA-7971-4A64-BD54-8A9F518CB4AD}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2565" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{69F113DC-7633-4730-BD7E-3337CEB2EA1E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{69F113DC-7633-4730-BD7E-3337CEB2EA1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Differential &amp; Integral" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="97">
   <si>
     <t>A Shim Rotation</t>
   </si>
@@ -208,7 +208,22 @@
     <t>E-661 I-1</t>
   </si>
   <si>
+    <t>Void V-23</t>
+  </si>
+  <si>
     <t>IX-45</t>
+  </si>
+  <si>
+    <t>E-660 V-23</t>
+  </si>
+  <si>
+    <t>E-661 V-23</t>
+  </si>
+  <si>
+    <t>Void IX-45</t>
+  </si>
+  <si>
+    <t>E-661 IX-45</t>
   </si>
   <si>
     <t>``</t>
@@ -303,12 +318,36 @@
   <si>
     <t>beta/l</t>
   </si>
+  <si>
+    <t>H wt%</t>
+  </si>
+  <si>
+    <t>H mass</t>
+  </si>
+  <si>
+    <t>Z wt%</t>
+  </si>
+  <si>
+    <t>Z-90 atomic density</t>
+  </si>
+  <si>
+    <t>Z-92 atomic density</t>
+  </si>
+  <si>
+    <t>Z-94 atomic density</t>
+  </si>
+  <si>
+    <t>Z-96 atomic density</t>
+  </si>
+  <si>
+    <t>Z-91 atomic density</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,6 +395,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -505,7 +552,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -536,6 +583,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -560,6 +608,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -775,40 +827,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.8591264160679195</c:v>
+                  <c:v>14.851977232236639</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.566764808416746</c:v>
+                  <c:v>7.7807123979966324</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5273104335142307</c:v>
+                  <c:v>3.4119860967612823</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.629059117286669</c:v>
+                  <c:v>8.4898654678227725</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.074003179927651</c:v>
+                  <c:v>18.718350288921279</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33.201521565081563</c:v>
+                  <c:v>26.706940142196419</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42.503079036840703</c:v>
+                  <c:v>36.375974446118654</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45.828608693272066</c:v>
+                  <c:v>39.110959116546084</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44.166329175258632</c:v>
+                  <c:v>41.262691764353441</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>33.373446658655489</c:v>
+                  <c:v>29.856930906026218</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19.604699994124541</c:v>
+                  <c:v>20.858394749046873</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10.637048677206002</c:v>
+                  <c:v>9.5732566172473526</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1081,37 +1133,37 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="12"/>
                       <c:pt idx="1">
-                        <c:v>70.470376209654887</c:v>
+                        <c:v>55.963492473789572</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>151.25222396365939</c:v>
+                        <c:v>115.47275029670985</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>334.76753544973099</c:v>
+                        <c:v>251.5138290804301</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>611.14515917477706</c:v>
+                        <c:v>478.64028123601861</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>989.66816218438839</c:v>
+                        <c:v>794.05485417759405</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>1431.3266008349524</c:v>
+                        <c:v>1171.4895219909176</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>1881.301290177606</c:v>
+                        <c:v>1573.3577763954154</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>2269.0001693471768</c:v>
+                        <c:v>1928.9558897473137</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>2533.8909026110769</c:v>
+                        <c:v>2182.5325180226791</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>2685.0996459677294</c:v>
+                        <c:v>2334.6907748541503</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>2738.2848893537594</c:v>
+                        <c:v>2382.557057940387</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1606,37 +1658,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>5.6956512418108103</c:v>
+                  <c:v>7.2939457405704164</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9358462411877557</c:v>
+                  <c:v>3.795520102077746</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.219151268439372</c:v>
+                  <c:v>7.3895502394577477</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.731180996682633</c:v>
+                  <c:v>12.52413979513384</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27.868065382961458</c:v>
+                  <c:v>23.751433828608324</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36.437969881787055</c:v>
+                  <c:v>29.102973807263588</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44.221516580808746</c:v>
+                  <c:v>40.184612517591383</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>47.774273282065302</c:v>
+                  <c:v>40.197627315844855</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>38.096398163309559</c:v>
+                  <c:v>33.172769324864319</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29.589002467320107</c:v>
+                  <c:v>29.645152160745965</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16.674782155027401</c:v>
+                  <c:v>20.250379958643226</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2339,37 +2391,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="2">
-                  <c:v>70.470376209654887</c:v>
+                  <c:v>55.963492473789572</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>151.25222396365939</c:v>
+                  <c:v>115.47275029670985</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>334.76753544973099</c:v>
+                  <c:v>251.5138290804301</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>611.14515917477706</c:v>
+                  <c:v>478.64028123601861</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>989.66816218438839</c:v>
+                  <c:v>794.05485417759405</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1431.3266008349524</c:v>
+                  <c:v>1171.4895219909176</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1881.301290177606</c:v>
+                  <c:v>1573.3577763954154</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2269.0001693471768</c:v>
+                  <c:v>1928.9558897473137</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2533.8909026110769</c:v>
+                  <c:v>2182.5325180226791</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2685.0996459677294</c:v>
+                  <c:v>2334.6907748541503</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2738.2848893537594</c:v>
+                  <c:v>2382.557057940387</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2695,38 +2747,44 @@
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="13"/>
+                      <c:pt idx="0">
+                        <c:v>51.34755033737698</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>139.16482937760605</c:v>
+                      </c:pt>
                       <c:pt idx="2">
-                        <c:v>53.157487414992829</c:v>
+                        <c:v>194.61215859084689</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>133.93247496312847</c:v>
+                        <c:v>250.53751029852435</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>268.6841362887385</c:v>
+                        <c:v>350.10596047148226</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>486.68036818695896</c:v>
+                        <c:v>531.48382859019307</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>808.21054451070154</c:v>
+                        <c:v>795.75586676955254</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>1211.5079768236806</c:v>
+                        <c:v>1142.1937983938274</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>1671.4869261380509</c:v>
+                        <c:v>1544.1049975610085</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>2100.8402833649252</c:v>
+                        <c:v>1910.9569807645544</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>2439.2672865180734</c:v>
+                        <c:v>2225.0465881926057</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>2670.586209629811</c:v>
+                        <c:v>2474.5242487895516</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>2753.9601204049482</c:v>
+                        <c:v>2575.7761485827677</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3264,38 +3322,44 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>51.34755033737698</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>139.16482937760605</c:v>
+                </c:pt>
                 <c:pt idx="2">
-                  <c:v>53.157487414992829</c:v>
+                  <c:v>194.61215859084689</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>133.93247496312847</c:v>
+                  <c:v>250.53751029852435</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>268.6841362887385</c:v>
+                  <c:v>350.10596047148226</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>486.68036818695896</c:v>
+                  <c:v>531.48382859019307</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>808.21054451070154</c:v>
+                  <c:v>795.75586676955254</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1211.5079768236806</c:v>
+                  <c:v>1142.1937983938274</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1671.4869261380509</c:v>
+                  <c:v>1544.1049975610085</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2100.8402833649252</c:v>
+                  <c:v>1910.9569807645544</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2439.2672865180734</c:v>
+                  <c:v>2225.0465881926057</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2670.586209629811</c:v>
+                  <c:v>2474.5242487895516</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2753.9601204049482</c:v>
+                  <c:v>2575.7761485827677</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -6501,49 +6565,50 @@
   <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="28.5">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
       <c r="F1" s="5"/>
       <c r="G1" s="6"/>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -6587,717 +6652,725 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>-20</v>
       </c>
-      <c r="B5">
-        <v>1.02136</v>
+      <c r="B5" s="8">
+        <v>0.99616099999999996</v>
       </c>
       <c r="C5">
         <f>(B5-1)/B5</f>
-        <v>2.0913292081146749E-2</v>
+        <v>-3.8537947179221399E-3</v>
       </c>
       <c r="D5">
         <f>C5*10^5</f>
-        <v>2091.3292081146751</v>
+        <v>-385.37947179221402</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
         <f>(E5+E6)/2*10</f>
-        <v>44.295632080339601</v>
+        <v>74.259886161183189</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5">
         <v>-20</v>
       </c>
-      <c r="I5">
-        <v>1.02454</v>
+      <c r="I5" s="8">
+        <v>0.99902400000000002</v>
       </c>
       <c r="J5">
         <f>(I5-1)/I5</f>
-        <v>2.3952212700333816E-2</v>
+        <v>-9.7695350662244042E-4</v>
       </c>
       <c r="K5">
         <f>J5*10^5</f>
-        <v>2395.2212700333816</v>
+        <v>-97.695350662244039</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
         <f>(L5+L6)/2*10</f>
-        <v>72.770528061853383</v>
+        <v>51.34755033737698</v>
+      </c>
+      <c r="N5">
+        <f>SUM($M$5:M5)</f>
+        <v>51.34755033737698</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>-10</v>
       </c>
-      <c r="B6">
-        <v>1.0222850000000001</v>
+      <c r="B6" s="8">
+        <v>0.997637</v>
       </c>
       <c r="C6">
         <f>(B6-1)/B6</f>
-        <v>2.1799204722753544E-2</v>
+        <v>-2.3685969946984765E-3</v>
       </c>
       <c r="D6">
         <f>C6*10^5</f>
-        <v>2179.9204722753543</v>
+        <v>-236.85969946984764</v>
       </c>
       <c r="E6">
         <f>ABS(D6-D5)/(10)</f>
-        <v>8.8591264160679195</v>
+        <v>14.851977232236639</v>
       </c>
       <c r="F6">
         <f t="shared" ref="F6:F16" si="0">(E6+E7)/2*10</f>
-        <v>107.12945612242333</v>
+        <v>113.16344815116636</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6">
         <v>-10</v>
       </c>
-      <c r="I6">
-        <v>1.02607</v>
+      <c r="I6" s="8">
+        <v>1.0000500000000001</v>
       </c>
       <c r="J6">
         <f>(I6-1)/I6</f>
-        <v>2.5407623261570884E-2</v>
+        <v>4.9997500125099255E-5</v>
       </c>
       <c r="K6">
         <f>J6*10^5</f>
-        <v>2540.7623261570884</v>
+        <v>4.9997500125099252</v>
       </c>
       <c r="L6">
         <f>ABS(K6-K5)/(H6-H5)</f>
-        <v>14.554105612370677</v>
+        <v>10.269510067475396</v>
       </c>
       <c r="M6">
         <f t="shared" ref="M6:M17" si="1">(L6+L7)/2*10</f>
-        <v>101.24878427090744</v>
+        <v>87.817279040229067</v>
+      </c>
+      <c r="N6">
+        <f>SUM($M$5:M6)</f>
+        <v>139.16482937760605</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0</v>
       </c>
-      <c r="B7">
-        <v>1.0236000000000001</v>
+      <c r="B7" s="8">
+        <v>0.99841199999999997</v>
       </c>
       <c r="C7">
         <f>(B7-1)/B7</f>
-        <v>2.3055881203595217E-2</v>
+        <v>-1.5905257548988131E-3</v>
       </c>
       <c r="D7">
         <f>C7*10^5</f>
-        <v>2305.5881203595218</v>
+        <v>-159.05257548988132</v>
       </c>
       <c r="E7">
         <f>ABS(D7-D6)/(A7-A6)</f>
-        <v>12.566764808416746</v>
+        <v>7.7807123979966324</v>
       </c>
       <c r="F7">
         <f>(E7+E8)/2*10</f>
-        <v>70.470376209654887</v>
+        <v>55.963492473789572</v>
       </c>
       <c r="G7" s="2">
         <f>SUM($F$7:F7)</f>
-        <v>70.470376209654887</v>
+        <v>55.963492473789572</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
-      <c r="I7">
-        <v>1.02667</v>
+      <c r="I7" s="8">
+        <v>1.00078</v>
       </c>
       <c r="J7">
         <f>(I7-1)/I7</f>
-        <v>2.5977188385751967E-2</v>
+        <v>7.7939207418214085E-4</v>
       </c>
       <c r="K7">
         <f>J7*10^5</f>
-        <v>2597.7188385751965</v>
+        <v>77.939207418214082</v>
       </c>
       <c r="L7">
         <f t="shared" ref="L7:L17" si="2">ABS(K7-K6)/(H7-H6)</f>
-        <v>5.6956512418108103</v>
+        <v>7.2939457405704164</v>
       </c>
       <c r="M7">
         <f t="shared" si="1"/>
-        <v>53.157487414992829</v>
+        <v>55.44732921324082</v>
       </c>
       <c r="N7">
-        <f>SUM($M$7:M7)</f>
-        <v>53.157487414992829</v>
+        <f>SUM($M$5:M7)</f>
+        <v>194.61215859084689</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>10</v>
       </c>
-      <c r="B8">
-        <v>1.0234399999999999</v>
+      <c r="B8" s="8">
+        <v>0.99807199999999996</v>
       </c>
       <c r="C8">
         <f>(B8-1)/B8</f>
-        <v>2.2903150160243795E-2</v>
+        <v>-1.9317243645749413E-3</v>
       </c>
       <c r="D8">
         <f>C8*10^5</f>
-        <v>2290.3150160243795</v>
+        <v>-193.17243645749414</v>
       </c>
       <c r="E8">
         <f t="shared" ref="E8:E17" si="3">ABS(D8-D7)/(A8-A7)</f>
-        <v>1.5273104335142307</v>
+        <v>3.4119860967612823</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>80.781847754004502</v>
+        <v>59.509257822920276</v>
       </c>
       <c r="G8" s="2">
         <f>SUM($F$7:F8)</f>
-        <v>151.25222396365939</v>
+        <v>115.47275029670985</v>
       </c>
       <c r="H8">
         <v>10</v>
       </c>
-      <c r="I8">
-        <v>1.0261499999999999</v>
+      <c r="I8" s="8">
+        <v>1.0004</v>
       </c>
       <c r="J8">
         <f>(I8-1)/I8</f>
-        <v>2.5483603761633191E-2</v>
+        <v>3.9984006397436622E-4</v>
       </c>
       <c r="K8">
         <f>J8*10^5</f>
-        <v>2548.360376163319</v>
+        <v>39.984006397436623</v>
       </c>
       <c r="L8">
         <f t="shared" si="2"/>
-        <v>4.9358462411877557</v>
+        <v>3.795520102077746</v>
       </c>
       <c r="M8">
         <f t="shared" si="1"/>
-        <v>80.774987548135641</v>
+        <v>55.925351707677464</v>
       </c>
       <c r="N8">
-        <f>SUM($M$7:M8)</f>
-        <v>133.93247496312847</v>
+        <f>SUM($M$5:M8)</f>
+        <v>250.53751029852435</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>20</v>
       </c>
-      <c r="B9">
-        <v>1.0219100000000001</v>
+      <c r="B9" s="8">
+        <v>0.99722699999999997</v>
       </c>
       <c r="C9">
         <f t="shared" ref="C9:C17" si="4">(B9-1)/B9</f>
-        <v>2.1440244248515129E-2</v>
+        <v>-2.7807109113572189E-3</v>
       </c>
       <c r="D9">
         <f t="shared" ref="D9:D17" si="5">C9*10^5</f>
-        <v>2144.0244248515128</v>
+        <v>-278.07109113572187</v>
       </c>
       <c r="E9">
         <f t="shared" si="3"/>
-        <v>14.629059117286669</v>
+        <v>8.4898654678227725</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>183.5153114860716</v>
+        <v>136.04107878372025</v>
       </c>
       <c r="G9" s="2">
         <f>SUM($F$7:F9)</f>
-        <v>334.76753544973099</v>
+        <v>251.5138290804301</v>
       </c>
       <c r="H9">
         <v>20</v>
       </c>
-      <c r="I9">
-        <v>1.0249699999999999</v>
+      <c r="I9" s="8">
+        <v>0.99966100000000002</v>
       </c>
       <c r="J9">
         <f t="shared" ref="J9:J17" si="6">(I9-1)/I9</f>
-        <v>2.4361688634789252E-2</v>
+        <v>-3.3911495997140852E-4</v>
       </c>
       <c r="K9">
         <f t="shared" ref="K9:K17" si="7">J9*10^5</f>
-        <v>2436.1688634789252</v>
+        <v>-33.911495997140854</v>
       </c>
       <c r="L9">
         <f t="shared" si="2"/>
-        <v>11.219151268439372</v>
+        <v>7.3895502394577477</v>
       </c>
       <c r="M9">
         <f t="shared" si="1"/>
-        <v>134.75166132561003</v>
+        <v>99.568450172957938</v>
       </c>
       <c r="N9">
-        <f>SUM($M$7:M9)</f>
-        <v>268.6841362887385</v>
+        <f>SUM($M$5:M9)</f>
+        <v>350.10596047148226</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>30</v>
       </c>
-      <c r="B10">
-        <v>1.0196099999999999</v>
+      <c r="B10" s="8">
+        <v>0.99536899999999995</v>
       </c>
       <c r="C10">
         <f t="shared" si="4"/>
-        <v>1.9232843930522363E-2</v>
+        <v>-4.6525459402493464E-3</v>
       </c>
       <c r="D10">
         <f t="shared" si="5"/>
-        <v>1923.2843930522363</v>
+        <v>-465.25459402493465</v>
       </c>
       <c r="E10">
         <f t="shared" si="3"/>
-        <v>22.074003179927651</v>
+        <v>18.718350288921279</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>276.37762372504608</v>
+        <v>227.12645215558851</v>
       </c>
       <c r="G10" s="2">
         <f>SUM($F$7:F10)</f>
-        <v>611.14515917477706</v>
+        <v>478.64028123601861</v>
       </c>
       <c r="H10">
         <v>30</v>
       </c>
-      <c r="I10">
-        <v>1.02332</v>
+      <c r="I10" s="8">
+        <v>0.99841100000000005</v>
       </c>
       <c r="J10">
         <f t="shared" si="6"/>
-        <v>2.2788570535120987E-2</v>
+        <v>-1.5915289394847927E-3</v>
       </c>
       <c r="K10">
         <f t="shared" si="7"/>
-        <v>2278.8570535120989</v>
+        <v>-159.15289394847926</v>
       </c>
       <c r="L10">
         <f t="shared" si="2"/>
-        <v>15.731180996682633</v>
+        <v>12.52413979513384</v>
       </c>
       <c r="M10">
         <f t="shared" si="1"/>
-        <v>217.99623189822046</v>
+        <v>181.37786811871081</v>
       </c>
       <c r="N10">
-        <f>SUM($M$7:M10)</f>
-        <v>486.68036818695896</v>
+        <f>SUM($M$5:M10)</f>
+        <v>531.48382859019307</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>40</v>
       </c>
-      <c r="B11">
-        <v>1.01617</v>
+      <c r="B11" s="8">
+        <v>0.99273</v>
       </c>
       <c r="C11">
         <f t="shared" si="4"/>
-        <v>1.5912691774014207E-2</v>
+        <v>-7.3232399544689878E-3</v>
       </c>
       <c r="D11">
         <f t="shared" si="5"/>
-        <v>1591.2691774014206</v>
+        <v>-732.32399544689883</v>
       </c>
       <c r="E11">
         <f t="shared" si="3"/>
-        <v>33.201521565081563</v>
+        <v>26.706940142196419</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>378.52300300961133</v>
+        <v>315.41457294157539</v>
       </c>
       <c r="G11" s="2">
         <f>SUM($F$7:F11)</f>
-        <v>989.66816218438839</v>
+        <v>794.05485417759405</v>
       </c>
       <c r="H11">
         <v>40</v>
       </c>
-      <c r="I11">
-        <v>1.02041</v>
+      <c r="I11" s="8">
+        <v>0.99604899999999996</v>
       </c>
       <c r="J11">
         <f t="shared" si="6"/>
-        <v>2.0001763996824844E-2</v>
+        <v>-3.9666723223456251E-3</v>
       </c>
       <c r="K11">
         <f t="shared" si="7"/>
-        <v>2000.1763996824843</v>
+        <v>-396.6672322345625</v>
       </c>
       <c r="L11">
         <f>ABS(K11-K10)/(H11-H10)</f>
-        <v>27.868065382961458</v>
+        <v>23.751433828608324</v>
       </c>
       <c r="M11">
         <f t="shared" si="1"/>
-        <v>321.53017632374258</v>
+        <v>264.27203817935953</v>
       </c>
       <c r="N11">
-        <f>SUM($M$7:M11)</f>
-        <v>808.21054451070154</v>
+        <f>SUM($M$5:M11)</f>
+        <v>795.75586676955254</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>50</v>
       </c>
-      <c r="B12">
-        <v>1.0118</v>
+      <c r="B12" s="8">
+        <v>0.98915799999999998</v>
       </c>
       <c r="C12">
         <f t="shared" si="4"/>
-        <v>1.1662383870330136E-2</v>
+        <v>-1.0960837399080853E-2</v>
       </c>
       <c r="D12">
         <f t="shared" si="5"/>
-        <v>1166.2383870330136</v>
+        <v>-1096.0837399080854</v>
       </c>
       <c r="E12">
         <f t="shared" si="3"/>
-        <v>42.503079036840703</v>
+        <v>36.375974446118654</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>441.65843865056388</v>
+        <v>377.4346678133237</v>
       </c>
       <c r="G12" s="2">
         <f>SUM($F$7:F12)</f>
-        <v>1431.3266008349524</v>
+        <v>1171.4895219909176</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
-      <c r="I12">
-        <v>1.0166299999999999</v>
+      <c r="I12" s="8">
+        <v>0.99317</v>
       </c>
       <c r="J12">
         <f t="shared" si="6"/>
-        <v>1.6357967008646137E-2</v>
+        <v>-6.8769697030719844E-3</v>
       </c>
       <c r="K12">
         <f t="shared" si="7"/>
-        <v>1635.7967008646137</v>
+        <v>-687.6969703071984</v>
       </c>
       <c r="L12">
         <f t="shared" si="2"/>
-        <v>36.437969881787055</v>
+        <v>29.102973807263588</v>
       </c>
       <c r="M12">
         <f t="shared" si="1"/>
-        <v>403.29743231297897</v>
+        <v>346.43793162427482</v>
       </c>
       <c r="N12">
-        <f>SUM($M$7:M12)</f>
-        <v>1211.5079768236806</v>
+        <f>SUM($M$5:M12)</f>
+        <v>1142.1937983938274</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>60</v>
       </c>
-      <c r="B13">
-        <v>1.0071300000000001</v>
+      <c r="B13" s="8">
+        <v>0.98534600000000006</v>
       </c>
       <c r="C13">
         <f t="shared" si="4"/>
-        <v>7.0795230010029294E-3</v>
+        <v>-1.4871933310735462E-2</v>
       </c>
       <c r="D13">
         <f t="shared" si="5"/>
-        <v>707.95230010029297</v>
+        <v>-1487.1933310735462</v>
       </c>
       <c r="E13">
         <f t="shared" si="3"/>
-        <v>45.828608693272066</v>
+        <v>39.110959116546084</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>449.97468934265351</v>
+        <v>401.86825440449763</v>
       </c>
       <c r="G13" s="2">
         <f>SUM($F$7:F13)</f>
-        <v>1881.301290177606</v>
+        <v>1573.3577763954154</v>
       </c>
       <c r="H13">
         <v>60</v>
       </c>
-      <c r="I13">
-        <v>1.0120800000000001</v>
+      <c r="I13" s="8">
+        <v>0.98922200000000005</v>
       </c>
       <c r="J13">
         <f t="shared" si="6"/>
-        <v>1.1935815350565262E-2</v>
+        <v>-1.0895430954831123E-2</v>
       </c>
       <c r="K13">
         <f t="shared" si="7"/>
-        <v>1193.5815350565263</v>
+        <v>-1089.5430954831122</v>
       </c>
       <c r="L13">
         <f>ABS(K13-K12)/(H13-H12)</f>
-        <v>44.221516580808746</v>
+        <v>40.184612517591383</v>
       </c>
       <c r="M13">
         <f t="shared" si="1"/>
-        <v>459.97894931437025</v>
+        <v>401.91119916718122</v>
       </c>
       <c r="N13">
-        <f>SUM($M$7:M13)</f>
-        <v>1671.4869261380509</v>
+        <f>SUM($M$5:M13)</f>
+        <v>1544.1049975610085</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>70</v>
       </c>
-      <c r="B14">
-        <v>1.00267</v>
+      <c r="B14" s="8">
+        <v>0.98135600000000001</v>
       </c>
       <c r="C14">
         <f t="shared" si="4"/>
-        <v>2.6628900834770666E-3</v>
+        <v>-1.8998202487170806E-2</v>
       </c>
       <c r="D14">
         <f t="shared" si="5"/>
-        <v>266.28900834770667</v>
+        <v>-1899.8202487170806</v>
       </c>
       <c r="E14">
         <f t="shared" si="3"/>
-        <v>44.166329175258632</v>
+        <v>41.262691764353441</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>387.6988791695706</v>
+        <v>355.59811335189829</v>
       </c>
       <c r="G14" s="2">
         <f>SUM($F$7:F14)</f>
-        <v>2269.0001693471768</v>
+        <v>1928.9558897473137</v>
       </c>
       <c r="H14">
         <v>70</v>
       </c>
-      <c r="I14">
-        <v>1.0072099999999999</v>
+      <c r="I14" s="8">
+        <v>0.98530399999999996</v>
       </c>
       <c r="J14">
         <f t="shared" si="6"/>
-        <v>7.1583880223587328E-3</v>
+        <v>-1.4915193686415607E-2</v>
       </c>
       <c r="K14">
         <f t="shared" si="7"/>
-        <v>715.83880223587323</v>
+        <v>-1491.5193686415607</v>
       </c>
       <c r="L14">
         <f t="shared" si="2"/>
-        <v>47.774273282065302</v>
+        <v>40.197627315844855</v>
       </c>
       <c r="M14">
         <f t="shared" si="1"/>
-        <v>429.35335722687427</v>
+        <v>366.85198320354584</v>
       </c>
       <c r="N14">
-        <f>SUM($M$7:M14)</f>
-        <v>2100.8402833649252</v>
+        <f>SUM($M$5:M14)</f>
+        <v>1910.9569807645544</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>80</v>
       </c>
-      <c r="B15">
-        <v>0.99932600000000005</v>
+      <c r="B15" s="8">
+        <v>0.97848900000000005</v>
       </c>
       <c r="C15">
         <f t="shared" si="4"/>
-        <v>-6.7445458238848217E-4</v>
+        <v>-2.198389557777343E-2</v>
       </c>
       <c r="D15">
         <f t="shared" si="5"/>
-        <v>-67.445458238848218</v>
+        <v>-2198.3895577773428</v>
       </c>
       <c r="E15">
         <f t="shared" si="3"/>
-        <v>33.373446658655489</v>
+        <v>29.856930906026218</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>264.89073326390013</v>
+        <v>253.57662827536544</v>
       </c>
       <c r="G15" s="2">
         <f>SUM($F$7:F15)</f>
-        <v>2533.8909026110769</v>
+        <v>2182.5325180226791</v>
       </c>
       <c r="H15">
         <v>80</v>
       </c>
-      <c r="I15">
-        <v>1.00336</v>
+      <c r="I15" s="8">
+        <v>0.98209400000000002</v>
       </c>
       <c r="J15">
         <f t="shared" si="6"/>
-        <v>3.3487482060277764E-3</v>
+        <v>-1.8232470618902038E-2</v>
       </c>
       <c r="K15">
         <f t="shared" si="7"/>
-        <v>334.87482060277762</v>
+        <v>-1823.2470618902039</v>
       </c>
       <c r="L15">
         <f t="shared" si="2"/>
-        <v>38.096398163309559</v>
+        <v>33.172769324864319</v>
       </c>
       <c r="M15">
         <f t="shared" si="1"/>
-        <v>338.42700315314829</v>
+        <v>314.08960742805141</v>
       </c>
       <c r="N15">
-        <f>SUM($M$7:M15)</f>
-        <v>2439.2672865180734</v>
+        <f>SUM($M$5:M15)</f>
+        <v>2225.0465881926057</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>90</v>
       </c>
-      <c r="B16">
-        <v>0.99737200000000004</v>
+      <c r="B16" s="8">
+        <v>0.97649600000000003</v>
       </c>
       <c r="C16">
         <f t="shared" si="4"/>
-        <v>-2.6349245818009363E-3</v>
+        <v>-2.4069735052678114E-2</v>
       </c>
       <c r="D16">
         <f t="shared" si="5"/>
-        <v>-263.49245818009365</v>
+        <v>-2406.9735052678116</v>
       </c>
       <c r="E16">
         <f t="shared" si="3"/>
-        <v>19.604699994124541</v>
+        <v>20.858394749046873</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>151.20874335665269</v>
+        <v>152.15825683147114</v>
       </c>
       <c r="G16" s="2">
         <f>SUM($F$7:F16)</f>
-        <v>2685.0996459677294</v>
+        <v>2334.6907748541503</v>
       </c>
       <c r="H16">
         <v>90</v>
       </c>
-      <c r="I16">
-        <v>1.0003899999999999</v>
+      <c r="I16" s="8">
+        <v>0.97924299999999997</v>
       </c>
       <c r="J16">
         <f t="shared" si="6"/>
-        <v>3.8984795929576513E-4</v>
+        <v>-2.1196985834976634E-2</v>
       </c>
       <c r="K16">
         <f t="shared" si="7"/>
-        <v>38.984795929576514</v>
+        <v>-2119.6985834976635</v>
       </c>
       <c r="L16">
         <f t="shared" si="2"/>
-        <v>29.589002467320107</v>
+        <v>29.645152160745965</v>
       </c>
       <c r="M16">
         <f t="shared" si="1"/>
-        <v>231.31892311173755</v>
+        <v>249.47766059694595</v>
       </c>
       <c r="N16">
-        <f>SUM($M$7:M16)</f>
-        <v>2670.586209629811</v>
+        <f>SUM($M$5:M16)</f>
+        <v>2474.5242487895516</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>100</v>
       </c>
-      <c r="B17" s="4">
-        <v>0.99631499999999995</v>
+      <c r="B17" s="20">
+        <v>0.97558400000000001</v>
       </c>
       <c r="C17" s="4">
         <f t="shared" si="4"/>
-        <v>-3.6986294495215365E-3</v>
+        <v>-2.5027060714402853E-2</v>
       </c>
       <c r="D17" s="4">
         <f t="shared" si="5"/>
-        <v>-369.86294495215367</v>
+        <v>-2502.7060714402851</v>
       </c>
       <c r="E17" s="4">
         <f t="shared" si="3"/>
-        <v>10.637048677206002</v>
+        <v>9.5732566172473526</v>
       </c>
       <c r="F17" s="4">
         <f>(E17+0)/2*10</f>
-        <v>53.18524338603001</v>
+        <v>47.866283086236763</v>
       </c>
       <c r="G17" s="2">
         <f>SUM($F$7:F17)</f>
-        <v>2738.2848893537594</v>
+        <v>2382.557057940387</v>
       </c>
       <c r="H17">
         <v>100</v>
       </c>
-      <c r="I17">
-        <v>0.99872399999999995</v>
+      <c r="I17" s="8">
+        <v>0.97730499999999998</v>
       </c>
       <c r="J17">
         <f t="shared" si="6"/>
-        <v>-1.277630256206975E-3</v>
+        <v>-2.3222023830840956E-2</v>
       </c>
       <c r="K17">
         <f t="shared" si="7"/>
-        <v>-127.7630256206975</v>
+        <v>-2322.2023830840958</v>
       </c>
       <c r="L17">
         <f t="shared" si="2"/>
-        <v>16.674782155027401</v>
+        <v>20.250379958643226</v>
       </c>
       <c r="M17">
         <f t="shared" si="1"/>
-        <v>83.373910775137006</v>
+        <v>101.25189979321613</v>
       </c>
       <c r="N17">
-        <f>SUM($M$7:M17)</f>
-        <v>2753.9601204049482</v>
+        <f>SUM($M$5:M17)</f>
+        <v>2575.7761485827677</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="28.5">
-      <c r="A21" s="20" t="s">
+    <row r="21" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="6"/>
-      <c r="J21" s="20" t="s">
+      <c r="J21" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
       <c r="R21" s="6"/>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -7353,7 +7426,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>0.14285714285714199</v>
       </c>
@@ -7419,7 +7492,7 @@
         <v>306.17631578947339</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>10.285714285714199</v>
       </c>
@@ -7485,7 +7558,7 @@
         <v>371.82894736842087</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>20.428571428571399</v>
       </c>
@@ -7551,7 +7624,7 @@
         <v>529.39526315789419</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>30.714285714285701</v>
       </c>
@@ -7617,7 +7690,7 @@
         <v>552.37368421052588</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>40.857142857142797</v>
       </c>
@@ -7683,7 +7756,7 @@
         <v>657.41789473684173</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>50.428571428571402</v>
       </c>
@@ -7749,7 +7822,7 @@
         <v>782.15789473684174</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>60.571428571428498</v>
       </c>
@@ -7815,7 +7888,7 @@
         <v>1231.8784210526255</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>70.428571428571402</v>
       </c>
@@ -7881,7 +7954,7 @@
         <v>1330.3573684210501</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>80.428571428571402</v>
       </c>
@@ -7947,7 +8020,7 @@
         <v>1524.0326315789421</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>90.142857142857096</v>
       </c>
@@ -8013,7 +8086,7 @@
         <v>1875.2742105263089</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>100.142857142857</v>
       </c>
@@ -8079,7 +8152,7 @@
         <v>2311.8642105263093</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="F34">
         <v>50.428571428571402</v>
@@ -8111,7 +8184,7 @@
         <v>2380.7994736842088</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="F35">
         <v>53.857142857142797</v>
@@ -8143,7 +8216,7 @@
         <v>2462.8652631578921</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="F36">
         <v>56.142857142857103</v>
@@ -8175,7 +8248,7 @@
         <v>2567.9094736842085</v>
       </c>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="F37">
         <v>72.285714285714207</v>
@@ -8207,7 +8280,7 @@
         <v>2672.9536842105254</v>
       </c>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="F38">
         <v>76.142857142857096</v>
@@ -8239,7 +8312,7 @@
         <v>2748.454210526309</v>
       </c>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="F39">
         <v>81.428571428571402</v>
@@ -8271,7 +8344,7 @@
         <v>2856.7810526315752</v>
       </c>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="F40">
         <v>88.142857142857096</v>
@@ -8290,7 +8363,7 @@
       <c r="J40" s="1"/>
       <c r="R40" s="2"/>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="F41">
         <v>98.428571428571402</v>
@@ -8309,7 +8382,7 @@
       <c r="J41" s="1"/>
       <c r="R41" s="2"/>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -8356,11 +8429,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A0E277-164D-40AC-8934-6E7AB0E9B78A}">
   <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:J8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:XFD48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
@@ -8368,58 +8441,61 @@
     <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="27" t="s">
+      <c r="G1" s="24"/>
+      <c r="H1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="M1" s="26" t="s">
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="M1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
     </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="F2" s="18" t="s">
         <v>24</v>
       </c>
@@ -8457,7 +8533,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>33</v>
       </c>
@@ -8518,7 +8594,7 @@
         <v>-24.927865646681809</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>37</v>
       </c>
@@ -8577,13 +8653,13 @@
         <f>Q4*100</f>
         <v>-83.94270568150398</v>
       </c>
-      <c r="S4" s="25" t="s">
+      <c r="S4" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="T4" s="25"/>
-      <c r="U4" s="25"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="26"/>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>40</v>
       </c>
@@ -8614,7 +8690,7 @@
         <v>63.950494478053749</v>
       </c>
       <c r="J5" s="15">
-        <f t="shared" ref="J5:J8" si="1">ABS(H5-F5)</f>
+        <f t="shared" ref="J5:J7" si="1">ABS(H5-F5)</f>
         <v>0.63565444323157738</v>
       </c>
       <c r="K5" s="15">
@@ -8642,13 +8718,13 @@
         <f>Q5*100</f>
         <v>-23.964483088892347</v>
       </c>
-      <c r="S5" s="25" t="s">
+      <c r="S5" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="T5" s="25"/>
-      <c r="U5" s="25"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>43</v>
       </c>
@@ -8693,22 +8769,22 @@
         <v>0.99841800000000003</v>
       </c>
       <c r="O6" s="8">
-        <f t="shared" ref="O6:O10" si="3">(N6-1)/N6</f>
+        <f t="shared" ref="O6:O14" si="3">(N6-1)/N6</f>
         <v>-1.5845066895828924E-3</v>
       </c>
       <c r="P6" s="8">
         <v>7.9256199999999995E-3</v>
       </c>
       <c r="Q6" s="8">
-        <f t="shared" ref="Q6:Q9" si="4">O6/P6</f>
+        <f t="shared" ref="Q6:Q14" si="4">O6/P6</f>
         <v>-0.19992211203450233</v>
       </c>
       <c r="R6">
-        <f t="shared" ref="R6:R9" si="5">Q6*100</f>
+        <f t="shared" ref="R6:R14" si="5">Q6*100</f>
         <v>-19.992211203450232</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>45</v>
       </c>
@@ -8768,7 +8844,7 @@
         <v>-22.343739422913444</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>47</v>
       </c>
@@ -8784,24 +8860,16 @@
       <c r="E8" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="15">
-        <v>0</v>
-      </c>
+      <c r="F8" s="15"/>
       <c r="G8" s="15">
         <v>11.5</v>
       </c>
-      <c r="H8" s="15">
-        <f>ABS(R9-R3)</f>
-        <v>47.45052758724519</v>
-      </c>
+      <c r="H8" s="15"/>
       <c r="I8" s="15">
         <f t="shared" si="0"/>
         <v>11.564312447576981</v>
       </c>
-      <c r="J8" s="15">
-        <f t="shared" si="1"/>
-        <v>47.45052758724519</v>
-      </c>
+      <c r="J8" s="15"/>
       <c r="K8" s="15">
         <f t="shared" si="2"/>
         <v>6.4312447576980958E-2</v>
@@ -8828,7 +8896,7 @@
         <v>-30.371104256255478</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>49</v>
       </c>
@@ -8844,16 +8912,20 @@
       <c r="E9" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="15">
-        <v>0</v>
-      </c>
+      <c r="F9" s="15"/>
       <c r="G9" s="15">
         <v>9</v>
       </c>
       <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
+      <c r="I9" s="15">
+        <f>ABS(R11-R10)</f>
+        <v>5.5444435315090317</v>
+      </c>
       <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
+      <c r="K9" s="15">
+        <f>ABS(I9-G9)</f>
+        <v>3.4555564684909683</v>
+      </c>
       <c r="M9" t="s">
         <v>51</v>
       </c>
@@ -8876,7 +8948,7 @@
         <v>-72.378393233927</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>47</v>
       </c>
@@ -8892,19 +8964,43 @@
       <c r="E10" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="15">
-        <v>0</v>
-      </c>
+      <c r="F10" s="15"/>
       <c r="G10" s="15">
         <v>10</v>
       </c>
       <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
+      <c r="I10" s="15">
+        <f>ABS(R12-R10)</f>
+        <v>9.0478486440546249</v>
+      </c>
       <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="O10" s="8"/>
+      <c r="K10" s="15">
+        <f>ABS(I10-G10)</f>
+        <v>0.95215135594537514</v>
+      </c>
+      <c r="M10" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="8">
+        <v>0.99401700000000004</v>
+      </c>
+      <c r="O10" s="8">
+        <f t="shared" si="3"/>
+        <v>-6.0190117472839599E-3</v>
+      </c>
+      <c r="P10" s="8">
+        <v>7.9182699999999998E-3</v>
+      </c>
+      <c r="Q10" s="8">
+        <f t="shared" si="4"/>
+        <v>-0.76014227189575001</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="5"/>
+        <v>-76.014227189574996</v>
+      </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>47</v>
       </c>
@@ -8918,57 +9014,152 @@
         <v>9.5399999999999991</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="15">
-        <v>0</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="F11" s="15"/>
       <c r="G11" s="15">
         <v>14.5</v>
       </c>
       <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
+      <c r="I11" s="15">
+        <f>ABS(R14-R13)</f>
+        <v>16.583190218726351</v>
+      </c>
       <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
+      <c r="K11" s="15">
+        <f>ABS(I11-G11)</f>
+        <v>2.0831902187263509</v>
+      </c>
+      <c r="M11" t="s">
+        <v>54</v>
+      </c>
+      <c r="N11" s="8">
+        <v>0.994448</v>
+      </c>
+      <c r="O11" s="8">
+        <f t="shared" si="3"/>
+        <v>-5.5829967982237395E-3</v>
+      </c>
+      <c r="P11" s="8">
+        <v>7.9225400000000005E-3</v>
+      </c>
+      <c r="Q11" s="8">
+        <f t="shared" si="4"/>
+        <v>-0.70469783658065965</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="5"/>
+        <v>-70.469783658065964</v>
+      </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N12" s="8">
+        <v>0.99470099999999995</v>
+      </c>
+      <c r="O12" s="8">
+        <f t="shared" si="3"/>
+        <v>-5.3272289863989823E-3</v>
+      </c>
+      <c r="P12" s="8">
+        <v>7.9550799999999998E-3</v>
+      </c>
+      <c r="Q12" s="8">
+        <f t="shared" si="4"/>
+        <v>-0.66966378545520377</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="5"/>
+        <v>-66.966378545520371</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M13" t="s">
+        <v>56</v>
+      </c>
+      <c r="N13" s="8">
+        <v>0.99488799999999999</v>
+      </c>
+      <c r="O13" s="8">
+        <f t="shared" si="3"/>
+        <v>-5.1382668199837622E-3</v>
+      </c>
+      <c r="P13" s="8">
+        <v>7.9193500000000003E-3</v>
+      </c>
+      <c r="Q13" s="8">
+        <f t="shared" si="4"/>
+        <v>-0.64882431259936257</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="5"/>
+        <v>-64.882431259936254</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N14" s="8">
+        <v>0.99618399999999996</v>
+      </c>
+      <c r="O14" s="8">
+        <f t="shared" si="3"/>
+        <v>-3.8306176369024615E-3</v>
+      </c>
+      <c r="P14" s="8">
+        <v>7.9310100000000005E-3</v>
+      </c>
+      <c r="Q14" s="8">
+        <f t="shared" si="4"/>
+        <v>-0.482992410412099</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="5"/>
+        <v>-48.299241041209903</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="23" t="s">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="23" t="s">
+      <c r="D24" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="23" t="s">
+      <c r="E24" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F24" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="G24" s="23"/>
-      <c r="H24" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
+      <c r="F24" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" s="24"/>
+      <c r="H24" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="N24" s="8"/>
     </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="25"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
       <c r="F25" s="18" t="s">
         <v>24</v>
       </c>
@@ -8982,13 +9173,13 @@
         <v>25</v>
       </c>
       <c r="J25" s="19" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="K25" s="19" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>33</v>
       </c>
@@ -9015,7 +9206,7 @@
         <f>ABS(R16-R16)</f>
         <v>0</v>
       </c>
-      <c r="I26" s="16">
+      <c r="I26" s="15">
         <f>(O3-O4)*10^5</f>
         <v>467.09085037238737</v>
       </c>
@@ -9028,7 +9219,7 @@
         <v>120.59085037238737</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>37</v>
       </c>
@@ -9056,7 +9247,7 @@
         <f>ABS(O5-$O$3)*10^5</f>
         <v>6.9266904923436865</v>
       </c>
-      <c r="I27" s="16">
+      <c r="I27" s="15">
         <f>(O5-$O$4)*10^5</f>
         <v>474.01754086473107</v>
       </c>
@@ -9069,7 +9260,7 @@
         <v>116.7375408647311</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>40</v>
       </c>
@@ -9094,15 +9285,15 @@
         <v>379.61</v>
       </c>
       <c r="H28" s="16">
-        <f t="shared" ref="H28:H34" si="7">ABS(O6-$O$3)*10^5</f>
+        <f t="shared" ref="H28:H30" si="7">ABS(O6-$O$3)*10^5</f>
         <v>38.235425845816039</v>
       </c>
-      <c r="I28" s="16">
+      <c r="I28" s="15">
         <f t="shared" ref="I28:I34" si="8">(O6-$O$4)*10^5</f>
         <v>505.32627621820336</v>
       </c>
       <c r="J28" s="15">
-        <f t="shared" ref="J28:J34" si="9">ABS(H28-F28)</f>
+        <f t="shared" ref="J28:J30" si="9">ABS(H28-F28)</f>
         <v>5.1254258458160393</v>
       </c>
       <c r="K28" s="15">
@@ -9110,7 +9301,7 @@
         <v>125.71627621820335</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>43</v>
       </c>
@@ -9138,7 +9329,7 @@
         <f t="shared" si="7"/>
         <v>19.974375330955866</v>
       </c>
-      <c r="I29" s="16">
+      <c r="I29" s="15">
         <f t="shared" si="8"/>
         <v>487.06522570334323</v>
       </c>
@@ -9151,7 +9342,7 @@
         <v>95.905225703343206</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>45</v>
       </c>
@@ -9179,7 +9370,7 @@
         <f t="shared" si="7"/>
         <v>43.187923722226095</v>
       </c>
-      <c r="I30" s="16">
+      <c r="I30" s="15">
         <f t="shared" si="8"/>
         <v>423.90292665016125</v>
       </c>
@@ -9192,7 +9383,7 @@
         <v>50.45292665016126</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>47</v>
       </c>
@@ -9208,19 +9399,13 @@
       <c r="E31" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F31" s="15">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
+      <c r="F31" s="15"/>
       <c r="G31" s="15">
         <f t="shared" si="6"/>
         <v>88.550000000000011</v>
       </c>
-      <c r="H31" s="16">
-        <f t="shared" si="7"/>
-        <v>377.18843325298741</v>
-      </c>
-      <c r="I31" s="16">
+      <c r="H31" s="16"/>
+      <c r="I31" s="15">
         <f t="shared" si="8"/>
         <v>89.902417119399999</v>
       </c>
@@ -9230,7 +9415,7 @@
         <v>1.3524171193999877</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>49</v>
       </c>
@@ -9246,29 +9431,23 @@
       <c r="E32" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="F32" s="15">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
+      <c r="F32" s="15"/>
       <c r="G32" s="15">
         <f t="shared" si="6"/>
         <v>69.3</v>
       </c>
-      <c r="H32" s="16">
-        <f t="shared" si="7"/>
-        <v>196.68609480410527</v>
-      </c>
-      <c r="I32" s="16">
+      <c r="H32" s="16"/>
+      <c r="I32" s="15">
         <f t="shared" si="8"/>
-        <v>663.77694517649263</v>
+        <v>61.875770448096681</v>
       </c>
       <c r="J32" s="15"/>
       <c r="K32" s="15">
         <f t="shared" si="10"/>
-        <v>594.47694517649268</v>
+        <v>7.4242295519033163</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
         <v>47</v>
       </c>
@@ -9284,29 +9463,23 @@
       <c r="E33" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="F33" s="15">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
+      <c r="F33" s="15"/>
       <c r="G33" s="15">
         <f t="shared" si="6"/>
         <v>77</v>
       </c>
-      <c r="H33" s="16">
-        <f t="shared" si="7"/>
-        <v>196.68609480410527</v>
-      </c>
-      <c r="I33" s="16">
+      <c r="H33" s="16"/>
+      <c r="I33" s="15">
         <f t="shared" si="8"/>
-        <v>663.77694517649263</v>
+        <v>105.47726535411871</v>
       </c>
       <c r="J33" s="15"/>
       <c r="K33" s="15">
         <f t="shared" si="10"/>
-        <v>586.77694517649263</v>
+        <v>28.477265354118714</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
         <v>47</v>
       </c>
@@ -9320,73 +9493,91 @@
         <v>9.5399999999999991</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="F34" s="15">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="F34" s="15"/>
       <c r="G34" s="15">
         <f t="shared" si="6"/>
         <v>111.64999999999999</v>
       </c>
-      <c r="H34" s="16">
-        <f t="shared" si="7"/>
-        <v>196.68609480410527</v>
-      </c>
-      <c r="I34" s="16">
+      <c r="H34" s="16"/>
+      <c r="I34" s="15">
         <f t="shared" si="8"/>
-        <v>663.77694517649263</v>
+        <v>131.05404653659443</v>
       </c>
       <c r="J34" s="15"/>
       <c r="K34" s="15">
         <f t="shared" si="10"/>
-        <v>552.12694517649265</v>
+        <v>19.404046536594436</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
-      <c r="A39" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C40" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D40" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="E40" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="F40" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="G40" t="s">
-        <v>65</v>
+        <v>67</v>
+      </c>
+      <c r="H40" t="s">
+        <v>92</v>
       </c>
       <c r="I40" t="s">
-        <v>66</v>
-      </c>
-      <c r="J40">
+        <v>96</v>
+      </c>
+      <c r="J40" t="s">
+        <v>93</v>
+      </c>
+      <c r="K40" t="s">
+        <v>94</v>
+      </c>
+      <c r="L40" t="s">
+        <v>95</v>
+      </c>
+      <c r="M40" t="s">
+        <v>68</v>
+      </c>
+      <c r="N40" t="s">
+        <v>69</v>
+      </c>
+      <c r="O40" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>71</v>
+      </c>
+      <c r="R40">
         <f>1E+24</f>
         <v>9.9999999999999998E+23</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B41">
         <v>309.63</v>
@@ -9395,26 +9586,53 @@
         <v>5.96</v>
       </c>
       <c r="D41">
+        <f>(C41*10^22)*1.00784*$R$47/$R$48</f>
+        <v>5.0866197943624272</v>
+      </c>
+      <c r="E41">
+        <f>D41/B41*100</f>
+        <v>1.6428058632440097</v>
+      </c>
+      <c r="F41">
+        <f>100-G41-E41</f>
+        <v>88.537194136756</v>
+      </c>
+      <c r="G41">
         <v>9.82</v>
       </c>
-      <c r="E41">
+      <c r="H41">
+        <v>1.83E-2</v>
+      </c>
+      <c r="I41">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J41">
+        <v>6.11E-3</v>
+      </c>
+      <c r="K41">
+        <v>6.1900000000000002E-3</v>
+      </c>
+      <c r="L41">
+        <v>9.9799999999999997E-4</v>
+      </c>
+      <c r="M41">
         <v>1.0399999999999999E-4</v>
       </c>
-      <c r="F41">
+      <c r="N41">
         <f>0.00143</f>
         <v>1.4300000000000001E-3</v>
       </c>
-      <c r="G41">
+      <c r="O41">
         <v>6.06</v>
       </c>
-      <c r="I41" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="J41" s="11">
+      <c r="Q41" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="R41" s="11">
         <v>2.54</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>37</v>
       </c>
@@ -9425,186 +9643,362 @@
         <v>5.97</v>
       </c>
       <c r="D42">
+        <f>(C42*10^22)*1.00784*$R$47/$R$48</f>
+        <v>5.0951543913328337</v>
+      </c>
+      <c r="E42">
+        <f t="shared" ref="E42:E49" si="11">D42/B42*100</f>
+        <v>1.64731794094175</v>
+      </c>
+      <c r="F42">
+        <f>100-G42-E42</f>
+        <v>88.65268205905825</v>
+      </c>
+      <c r="G42">
         <v>9.6999999999999993</v>
       </c>
-      <c r="E42">
-        <f t="shared" ref="E42:F49" si="11">E$41*$D42/$D$41</f>
+      <c r="H42">
+        <f>H$41*$F42/$F$41</f>
+        <v>1.8323870521296019E-2</v>
+      </c>
+      <c r="I42">
+        <f t="shared" ref="I42:L49" si="12">I$41*$F42/$F$41</f>
+        <v>4.0052176002832833E-3</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="12"/>
+        <v>6.1179698844327146E-3</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="12"/>
+        <v>6.1980742364383798E-3</v>
+      </c>
+      <c r="L42">
+        <f>L$41*$F42/$F$41</f>
+        <v>9.9930179127067894E-4</v>
+      </c>
+      <c r="M42">
+        <f>M$41*$G42/$G$41</f>
         <v>1.0272912423625252E-4</v>
       </c>
-      <c r="F42">
-        <f t="shared" si="11"/>
+      <c r="N42">
+        <f>N$41*$G42/$G$41</f>
         <v>1.4125254582484723E-3</v>
       </c>
-      <c r="G42">
-        <f t="shared" ref="G42:G49" si="12">B42/$J$47</f>
+      <c r="O42">
+        <f>B42/$R$47</f>
         <v>6.0650947308232492</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
-      <c r="A43" t="s">
+    <row r="43" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B43" s="32">
         <v>311.5</v>
       </c>
       <c r="C43" s="10">
         <v>6.27</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="31">
+        <f>(C43*10^22)*1.00784*$R$47/$R$48</f>
+        <v>5.3511923004450361</v>
+      </c>
+      <c r="E43" s="31">
+        <f t="shared" si="11"/>
+        <v>1.7178787481364481</v>
+      </c>
+      <c r="F43" s="31">
+        <f>100-G43-E43</f>
+        <v>88.332121251863555</v>
+      </c>
+      <c r="G43" s="31">
         <v>9.9499999999999993</v>
       </c>
-      <c r="E43">
-        <f t="shared" si="11"/>
+      <c r="H43" s="31">
+        <f t="shared" ref="H43:H49" si="13">H$41*$F43/$F$41</f>
+        <v>1.8257612912515219E-2</v>
+      </c>
+      <c r="I43" s="31">
+        <f t="shared" si="12"/>
+        <v>3.9907350628448565E-3</v>
+      </c>
+      <c r="J43" s="31">
+        <f t="shared" si="12"/>
+        <v>6.0958478084955177E-3</v>
+      </c>
+      <c r="K43" s="31">
+        <f t="shared" si="12"/>
+        <v>6.1756625097524158E-3</v>
+      </c>
+      <c r="L43" s="31">
+        <f t="shared" si="12"/>
+        <v>9.9568839817979165E-4</v>
+      </c>
+      <c r="M43" s="31">
+        <f>M$41*$G43/$G$41</f>
         <v>1.0537678207739306E-4</v>
       </c>
-      <c r="F43">
-        <f t="shared" si="11"/>
+      <c r="N43" s="31">
+        <f>N$41*$G43/$G$41</f>
         <v>1.4489307535641546E-3</v>
       </c>
-      <c r="G43">
-        <f t="shared" si="12"/>
+      <c r="O43" s="31">
+        <f>B43/$R$47</f>
         <v>6.1082347515403885</v>
       </c>
-      <c r="I43" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="J43" s="11">
+      <c r="Q43" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="R43" s="11">
         <f>0.532/2</f>
         <v>0.26600000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
-      <c r="A44" t="s">
+    <row r="44" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="31">
         <v>317.3</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="31">
         <v>5.97</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="31">
+        <f>(C44*10^22)*1.00784*$R$47/$R$48</f>
+        <v>5.0951543913328337</v>
+      </c>
+      <c r="E44" s="31">
+        <f t="shared" si="11"/>
+        <v>1.6057845544698499</v>
+      </c>
+      <c r="F44" s="31">
+        <f>100-G44-E44</f>
+        <v>88.284215445530151</v>
+      </c>
+      <c r="G44" s="31">
         <v>10.11</v>
       </c>
-      <c r="E44">
+      <c r="H44" s="31">
+        <f>H$41*$F44/$F$41</f>
+        <v>1.8247711127571061E-2</v>
+      </c>
+      <c r="I44" s="31">
+        <f t="shared" si="12"/>
+        <v>3.9885707382668984E-3</v>
+      </c>
+      <c r="J44" s="31">
+        <f>J$41*$F44/$F$41</f>
+        <v>6.0925418027026872E-3</v>
+      </c>
+      <c r="K44" s="31">
+        <f>K$41*$F44/$F$41</f>
+        <v>6.1723132174680258E-3</v>
+      </c>
+      <c r="L44" s="31">
+        <f t="shared" si="12"/>
+        <v>9.9514839919759117E-4</v>
+      </c>
+      <c r="M44" s="31">
+        <f>M$41*$G44/$G$41</f>
+        <v>1.0707128309572299E-4</v>
+      </c>
+      <c r="N44" s="31">
+        <f>N$41*$G44/$G$41</f>
+        <v>1.4722301425661914E-3</v>
+      </c>
+      <c r="O44" s="31">
+        <f>B44/$R$47</f>
+        <v>6.2219675334310285</v>
+      </c>
+      <c r="Q44" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="R44" s="11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="31">
+        <v>293.89999999999998</v>
+      </c>
+      <c r="C45" s="31">
+        <v>6.15</v>
+      </c>
+      <c r="D45" s="31">
+        <f>(C45*10^22)*1.00784*$R$47/$R$48</f>
+        <v>5.2487771368001548</v>
+      </c>
+      <c r="E45" s="31">
         <f t="shared" si="11"/>
-        <v>1.0707128309572299E-4</v>
-      </c>
-      <c r="F44">
-        <f t="shared" si="11"/>
-        <v>1.4722301425661914E-3</v>
-      </c>
-      <c r="G44">
+        <v>1.7859057968016858</v>
+      </c>
+      <c r="F45" s="31">
+        <f>100-G45-E45</f>
+        <v>88.894094203198321</v>
+      </c>
+      <c r="G45" s="31">
+        <v>9.32</v>
+      </c>
+      <c r="H45" s="31">
+        <f t="shared" si="13"/>
+        <v>1.837376867179466E-2</v>
+      </c>
+      <c r="I45" s="31">
+        <f>I$41*$F45/$F$41</f>
+        <v>4.0161242998458272E-3</v>
+      </c>
+      <c r="J45" s="31">
         <f t="shared" si="12"/>
-        <v>6.2219675334310285</v>
-      </c>
-      <c r="I44" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J44" s="11">
-        <v>14</v>
+        <v>6.1346298680145014E-3</v>
+      </c>
+      <c r="K45" s="31">
+        <f t="shared" si="12"/>
+        <v>6.2149523540114176E-3</v>
+      </c>
+      <c r="L45" s="31">
+        <f t="shared" si="12"/>
+        <v>1.0020230128115341E-3</v>
+      </c>
+      <c r="M45" s="31">
+        <f>M$41*$G45/$G$41</f>
+        <v>9.8704684317718941E-5</v>
+      </c>
+      <c r="N45" s="31">
+        <f>N$41*$G45/$G$41</f>
+        <v>1.3571894093686355E-3</v>
+      </c>
+      <c r="O45" s="31">
+        <f>B45/$R$47</f>
+        <v>5.7631145858032751</v>
+      </c>
+      <c r="Q45" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="R45" s="11">
+        <f>R43*R41</f>
+        <v>0.67564000000000002</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
-      <c r="A45" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45">
-        <v>293.89999999999998</v>
-      </c>
-      <c r="C45">
-        <v>6.15</v>
-      </c>
-      <c r="D45">
-        <v>9.32</v>
-      </c>
-      <c r="E45">
-        <f t="shared" si="11"/>
-        <v>9.8704684317718941E-5</v>
-      </c>
-      <c r="F45">
-        <f t="shared" si="11"/>
-        <v>1.3571894093686355E-3</v>
-      </c>
-      <c r="G45">
+    <row r="46" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="31">
+        <v>278</v>
+      </c>
+      <c r="C46" s="31">
+        <v>0</v>
+      </c>
+      <c r="F46" s="31">
+        <f>100-G46-E46</f>
+        <v>90.460000000000008</v>
+      </c>
+      <c r="G46" s="31">
+        <v>9.5399999999999991</v>
+      </c>
+      <c r="H46" s="31">
+        <f t="shared" si="13"/>
+        <v>1.8697430115562672E-2</v>
+      </c>
+      <c r="I46" s="31">
+        <f>I$41*$F46/$F$41</f>
+        <v>4.0868699706147907E-3</v>
+      </c>
+      <c r="J46" s="31">
         <f t="shared" si="12"/>
-        <v>5.7631145858032751</v>
-      </c>
-      <c r="I45" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="J45" s="11">
-        <f>J43*J41</f>
-        <v>0.67564000000000002</v>
+        <v>6.2426938801140933E-3</v>
+      </c>
+      <c r="K46" s="31">
+        <f t="shared" si="12"/>
+        <v>6.3244312795263892E-3</v>
+      </c>
+      <c r="L46" s="31">
+        <f t="shared" si="12"/>
+        <v>1.0196740576683904E-3</v>
+      </c>
+      <c r="M46" s="31">
+        <f>M$41*$G46/$G$41</f>
+        <v>1.0103462321792258E-4</v>
+      </c>
+      <c r="N46" s="31">
+        <f>N$41*$G46/$G$41</f>
+        <v>1.3892260692464358E-3</v>
+      </c>
+      <c r="O46" s="31">
+        <f>B46/$R$47</f>
+        <v>5.4513298906203147</v>
+      </c>
+      <c r="Q46" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="R46" s="11">
+        <f>R44*R41</f>
+        <v>35.56</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
-      <c r="A46" t="s">
-        <v>47</v>
-      </c>
-      <c r="B46">
-        <v>278</v>
-      </c>
-      <c r="C46">
+    <row r="47" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="29">
+        <v>278.3</v>
+      </c>
+      <c r="C47" s="29">
         <v>0</v>
       </c>
-      <c r="D46">
-        <v>9.5399999999999991</v>
-      </c>
-      <c r="E46">
-        <f t="shared" si="11"/>
-        <v>1.0103462321792258E-4</v>
-      </c>
-      <c r="F46">
-        <f t="shared" si="11"/>
-        <v>1.3892260692464358E-3</v>
-      </c>
-      <c r="G46">
+      <c r="F47" s="29">
+        <f>100-G47-E47</f>
+        <v>90.22</v>
+      </c>
+      <c r="G47" s="29">
+        <v>9.7799999999999994</v>
+      </c>
+      <c r="H47" s="29">
+        <f t="shared" si="13"/>
+        <v>1.8647823845081405E-2</v>
+      </c>
+      <c r="I47" s="29">
         <f t="shared" si="12"/>
-        <v>5.4513298906203147</v>
-      </c>
-      <c r="I46" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="J46" s="11">
-        <f>J44*J41</f>
-        <v>35.56</v>
+        <v>4.0760270699631484E-3</v>
+      </c>
+      <c r="J47" s="29">
+        <f t="shared" si="12"/>
+        <v>6.2261313493687086E-3</v>
+      </c>
+      <c r="K47" s="29">
+        <f t="shared" si="12"/>
+        <v>6.3076518907679725E-3</v>
+      </c>
+      <c r="L47" s="29">
+        <f t="shared" si="12"/>
+        <v>1.0169687539558054E-3</v>
+      </c>
+      <c r="M47" s="29">
+        <f>M$41*$G47/$G$41</f>
+        <v>1.0357637474541749E-4</v>
+      </c>
+      <c r="N47" s="29">
+        <f>N$41*$G47/$G$41</f>
+        <v>1.4241751527494908E-3</v>
+      </c>
+      <c r="O47" s="29">
+        <f>B47/$R$47</f>
+        <v>5.4572126207181064</v>
+      </c>
+      <c r="Q47" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="R47" s="30">
+        <f>PI()*R45^2*R46</f>
+        <v>50.996730261790482</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
-      <c r="A47" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47">
-        <v>278.3</v>
-      </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
-      <c r="D47">
-        <v>9.7799999999999994</v>
-      </c>
-      <c r="E47">
-        <f t="shared" si="11"/>
-        <v>1.0357637474541749E-4</v>
-      </c>
-      <c r="F47">
-        <f t="shared" si="11"/>
-        <v>1.4241751527494908E-3</v>
-      </c>
-      <c r="G47">
-        <f t="shared" si="12"/>
-        <v>5.4572126207181064</v>
-      </c>
-      <c r="I47" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="J47" s="11">
-        <f>PI()*J45^2*J46</f>
-        <v>50.996730261790482</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -9614,30 +10008,54 @@
       <c r="C48">
         <v>0</v>
       </c>
-      <c r="D48">
+      <c r="F48">
+        <f>100-G48-E48</f>
+        <v>90.460000000000008</v>
+      </c>
+      <c r="G48">
         <v>9.5399999999999991</v>
       </c>
-      <c r="E48">
-        <f t="shared" si="11"/>
+      <c r="H48">
+        <f t="shared" si="13"/>
+        <v>1.8697430115562672E-2</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="12"/>
+        <v>4.0868699706147907E-3</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="12"/>
+        <v>6.2426938801140933E-3</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="12"/>
+        <v>6.3244312795263892E-3</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="12"/>
+        <v>1.0196740576683904E-3</v>
+      </c>
+      <c r="M48">
+        <f>M$41*$G48/$G$41</f>
         <v>1.0103462321792258E-4</v>
       </c>
-      <c r="F48">
-        <f t="shared" si="11"/>
+      <c r="N48">
+        <f>N$41*$G48/$G$41</f>
         <v>1.3892260692464358E-3</v>
       </c>
-      <c r="G48">
-        <f t="shared" si="12"/>
+      <c r="O48">
+        <f>B48/$R$47</f>
         <v>5.4513298906203147</v>
       </c>
-      <c r="I48" t="s">
-        <v>74</v>
-      </c>
-      <c r="J48">
+      <c r="Q48" t="s">
+        <v>79</v>
+      </c>
+      <c r="R48">
         <f>6.0221408E+23</f>
         <v>6.0221408E+23</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -9647,25 +10065,49 @@
       <c r="C49">
         <v>0</v>
       </c>
-      <c r="D49">
+      <c r="F49">
+        <f>100-G49-E49</f>
+        <v>90.460000000000008</v>
+      </c>
+      <c r="G49">
         <v>9.5399999999999991</v>
       </c>
-      <c r="E49">
-        <f t="shared" si="11"/>
+      <c r="H49">
+        <f t="shared" si="13"/>
+        <v>1.8697430115562672E-2</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="12"/>
+        <v>4.0868699706147907E-3</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="12"/>
+        <v>6.2426938801140933E-3</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="12"/>
+        <v>6.3244312795263892E-3</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="12"/>
+        <v>1.0196740576683904E-3</v>
+      </c>
+      <c r="M49">
+        <f>M$41*$G49/$G$41</f>
         <v>1.0103462321792258E-4</v>
       </c>
-      <c r="F49">
-        <f t="shared" si="11"/>
+      <c r="N49">
+        <f>N$41*$G49/$G$41</f>
         <v>1.3892260692464358E-3</v>
       </c>
-      <c r="G49">
-        <f t="shared" si="12"/>
+      <c r="O49">
+        <f>B49/$R$47</f>
         <v>5.4513298906203147</v>
       </c>
-      <c r="I49" t="s">
-        <v>75</v>
-      </c>
-      <c r="J49">
+      <c r="Q49" t="s">
+        <v>80</v>
+      </c>
+      <c r="R49">
         <v>6.06</v>
       </c>
     </row>
@@ -9703,7 +10145,7 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
@@ -9713,26 +10155,26 @@
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B3">
         <f>0.00797</f>
@@ -9749,9 +10191,9 @@
         <v>26.99999999999994</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B4" s="9">
         <v>6.8426399999999998E-6</v>
@@ -9768,9 +10210,9 @@
         <v>15.52296296296297</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B5">
         <f>B3/B4</f>
@@ -9791,10 +10233,10 @@
         <v>214.75512375340509</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" s="13"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -9806,6 +10248,33 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e1ecaa1f-5549-4843-8e0b-36d11b9c4a00" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02f07221-7782-4248-899f-09bd431cf93f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="e1ecaa1f-5549-4843-8e0b-36d11b9c4a00">
+      <UserInfo>
+        <DisplayName>Oliver Douglas Paleen</DisplayName>
+        <AccountId>61</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ABEDCDC6898E9D48B17B2D917023A0E9" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c9b35f98bcdb4a0d7929321150581d5e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="02f07221-7782-4248-899f-09bd431cf93f" xmlns:ns3="e1ecaa1f-5549-4843-8e0b-36d11b9c4a00" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="53fe39de12092328c3276185799bfa71" ns2:_="" ns3:_="">
     <xsd:import namespace="02f07221-7782-4248-899f-09bd431cf93f"/>
@@ -10042,41 +10511,46 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e1ecaa1f-5549-4843-8e0b-36d11b9c4a00" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02f07221-7782-4248-899f-09bd431cf93f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="e1ecaa1f-5549-4843-8e0b-36d11b9c4a00">
-      <UserInfo>
-        <DisplayName>Oliver Douglas Paleen</DisplayName>
-        <AccountId>61</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4FEB34B-0950-495E-8A7D-7F2024A133DD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A981A7-99F7-420B-92E3-468028514462}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="02f07221-7782-4248-899f-09bd431cf93f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="e1ecaa1f-5549-4843-8e0b-36d11b9c4a00"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A981A7-99F7-420B-92E3-468028514462}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC7DCD2E-E082-4B2B-AAD1-C045E4862869}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC7DCD2E-E082-4B2B-AAD1-C045E4862869}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4FEB34B-0950-495E-8A7D-7F2024A133DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="02f07221-7782-4248-899f-09bd431cf93f"/>
+    <ds:schemaRef ds:uri="e1ecaa1f-5549-4843-8e0b-36d11b9c4a00"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[DOC & DEV] Updates to excel sheet, some graphing scripts and milestone
</commit_message>
<xml_diff>
--- a/snapReactors/reference_calc/DryExperiments.xlsx
+++ b/snapReactors/reference_calc/DryExperiments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4761bce209af5ea/Documents/SNAP-REACTORS/snapReactors/reference_calc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Documents\SNAP-REACTORS\snapReactors\reference_calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2819" documentId="8_{BEA5E111-021F-45DA-85BB-227D92BE1F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69B770FC-C7EF-4A4B-801D-640EA050BF8A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD71D7C9-E116-4ED0-94A6-47BF9A9E4DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{69F113DC-7633-4730-BD7E-3337CEB2EA1E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="5" activeTab="7" xr2:uid="{69F113DC-7633-4730-BD7E-3337CEB2EA1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Differential &amp; Integral Worth" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="188">
   <si>
     <t>A Shim Rotation (Drum 6)</t>
   </si>
@@ -642,15 +642,31 @@
   <si>
     <t>C-4 Base Case</t>
   </si>
+  <si>
+    <t>Total A Worth</t>
+  </si>
+  <si>
+    <t>Single A Shim Worth</t>
+  </si>
+  <si>
+    <t>B-Shim Removed</t>
+  </si>
+  <si>
+    <t>Modeled Six Shim Worth [pcm]</t>
+  </si>
+  <si>
+    <t>Modeled uncertainty [pcm]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -995,7 +1011,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -1074,6 +1090,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1090,18 +1109,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -10933,6 +10952,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -11232,64 +11255,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B7A4BB-76B8-4F5C-9E59-B1DED5EC6FFB}">
   <dimension ref="A1:AH57"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O61" sqref="O61"/>
+    <sheetView topLeftCell="S1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AB5" sqref="AB5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.1328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="42.1328125" customWidth="1"/>
-    <col min="25" max="25" width="27.265625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="27.265625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.73046875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="24.59765625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="27.265625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="42.140625" customWidth="1"/>
+    <col min="25" max="25" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="28.5">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:31" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
       <c r="F1" s="5"/>
       <c r="G1" s="6"/>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="T1" s="50" t="s">
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="T1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
+      <c r="U1" s="52"/>
+      <c r="V1" s="52"/>
+      <c r="W1" s="52"/>
+      <c r="X1" s="52"/>
       <c r="Y1" s="24"/>
       <c r="Z1" s="24"/>
       <c r="AA1" s="24"/>
@@ -11298,19 +11321,19 @@
       <c r="AD1" s="24"/>
       <c r="AE1" s="25"/>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="G2" s="2"/>
       <c r="T2" s="26"/>
       <c r="AE2" s="27"/>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="G3" s="2"/>
       <c r="T3" s="26"/>
       <c r="AE3" s="27"/>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -11390,7 +11413,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>-20</v>
       </c>
@@ -11448,7 +11471,7 @@
         <v>4.6E-5</v>
       </c>
       <c r="W5" s="8">
-        <f t="shared" ref="W5:W18" si="0">(U5-1)/U5</f>
+        <f>(U5-1)/U5</f>
         <v>-3.7493995503501056E-2</v>
       </c>
       <c r="X5" s="8">
@@ -11456,14 +11479,14 @@
         <v>4.9514114372467652</v>
       </c>
       <c r="Y5">
-        <f t="shared" ref="Y5:Y18" si="1">W5*10^5</f>
+        <f t="shared" ref="Y5:Y18" si="0">W5*10^5</f>
         <v>-3749.3995503501055</v>
       </c>
       <c r="Z5">
         <v>0</v>
       </c>
       <c r="AB5">
-        <f t="shared" ref="AB5:AB17" si="2">(Z5+Z6)/2*ABS(T6-T5)</f>
+        <f>(Z5+Z6)/2*ABS(T6-T5)</f>
         <v>6.7803945195066717</v>
       </c>
       <c r="AC5">
@@ -11472,7 +11495,7 @@
       </c>
       <c r="AE5" s="27"/>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>-10</v>
       </c>
@@ -11492,7 +11515,7 @@
         <v>14.851977232236639</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F16" si="3">(E6+E7)/2*10</f>
+        <f t="shared" ref="F6:F16" si="1">(E6+E7)/2*10</f>
         <v>113.16344815116636</v>
       </c>
       <c r="G6" s="2"/>
@@ -11515,7 +11538,7 @@
         <v>10.269510067475396</v>
       </c>
       <c r="M6">
-        <f t="shared" ref="M6:M17" si="4">(L6+L7)/2*10</f>
+        <f t="shared" ref="M6:M17" si="2">(L6+L7)/2*10</f>
         <v>87.817279040229067</v>
       </c>
       <c r="N6">
@@ -11532,19 +11555,19 @@
         <v>4.8000000000000001E-5</v>
       </c>
       <c r="W6">
+        <f t="shared" ref="W6:W18" si="3">(U6-1)/U6</f>
+        <v>-3.7358387613110923E-2</v>
+      </c>
+      <c r="X6" s="8">
+        <f t="shared" ref="X6:X18" si="4">V6/U6^2*10^5</f>
+        <v>5.1653396368861122</v>
+      </c>
+      <c r="Y6">
         <f t="shared" si="0"/>
-        <v>-3.7358387613110923E-2</v>
-      </c>
-      <c r="X6" s="8">
-        <f t="shared" ref="X6:X18" si="5">V6/U6^2*10^5</f>
-        <v>5.1653396368861122</v>
-      </c>
-      <c r="Y6">
-        <f t="shared" si="1"/>
         <v>-3735.8387613110922</v>
       </c>
       <c r="Z6">
-        <f t="shared" ref="Z6:Z18" si="6">ABS(Y6-Y5)/ABS(T6-T5)</f>
+        <f>ABS(Y6-Y5)/ABS(T6-T5)</f>
         <v>1.3560789039013343</v>
       </c>
       <c r="AA6">
@@ -11552,16 +11575,16 @@
         <v>0.71552224832834399</v>
       </c>
       <c r="AB6">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="AB6:AB17" si="5">(Z6+Z7)/2*ABS(T7-T6)</f>
         <v>36.302867231748678</v>
       </c>
       <c r="AC6">
-        <f t="shared" ref="AC6:AC17" si="7">SQRT((AA6*ABS(T7-T6)/2)^2+(AA7*ABS(T7-T6)/2)^2)</f>
+        <f t="shared" ref="AC6:AC17" si="6">SQRT((AA6*ABS(T7-T6)/2)^2+(AA7*ABS(T7-T6)/2)^2)</f>
         <v>5.1385480629455644</v>
       </c>
       <c r="AE6" s="27"/>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -11603,11 +11626,11 @@
         <v>77.939207418214082</v>
       </c>
       <c r="L7">
-        <f t="shared" ref="L7:L17" si="8">ABS(K7-K6)/(H7-H6)</f>
+        <f t="shared" ref="L7:L17" si="7">ABS(K7-K6)/(H7-H6)</f>
         <v>7.2939457405704164</v>
       </c>
       <c r="M7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>55.44732921324082</v>
       </c>
       <c r="N7">
@@ -11624,19 +11647,19 @@
         <v>4.8999999999999998E-5</v>
       </c>
       <c r="W7">
+        <f t="shared" si="3"/>
+        <v>-3.676793815886608E-2</v>
+      </c>
+      <c r="X7" s="8">
+        <f t="shared" si="4"/>
+        <v>5.2669500122115132</v>
+      </c>
+      <c r="Y7">
         <f t="shared" si="0"/>
-        <v>-3.676793815886608E-2</v>
-      </c>
-      <c r="X7" s="8">
-        <f t="shared" si="5"/>
-        <v>5.2669500122115132</v>
-      </c>
-      <c r="Y7">
-        <f t="shared" si="1"/>
         <v>-3676.7938158866082</v>
       </c>
       <c r="Z7">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="Z7:Z18" si="8">ABS(Y7-Y6)/ABS(T7-T6)</f>
         <v>5.9044945424484014</v>
       </c>
       <c r="AA7">
@@ -11644,11 +11667,11 @@
         <v>0.73770926519545366</v>
       </c>
       <c r="AB7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>70.175068824835535</v>
       </c>
       <c r="AC7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>5.1866346924367912</v>
       </c>
       <c r="AD7">
@@ -11660,7 +11683,7 @@
         <v>5.1866346924367912</v>
       </c>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>10</v>
       </c>
@@ -11680,7 +11703,7 @@
         <v>3.4119860967612823</v>
       </c>
       <c r="F8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>59.509257822920276</v>
       </c>
       <c r="G8" s="2">
@@ -11702,11 +11725,11 @@
         <v>39.984006397436623</v>
       </c>
       <c r="L8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>3.795520102077746</v>
       </c>
       <c r="M8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>55.925351707677464</v>
       </c>
       <c r="N8">
@@ -11723,19 +11746,19 @@
         <v>4.6999999999999997E-5</v>
       </c>
       <c r="W8">
+        <f t="shared" si="3"/>
+        <v>-3.5954886236614213E-2</v>
+      </c>
+      <c r="X8" s="8">
+        <f t="shared" si="4"/>
+        <v>5.0440518736923261</v>
+      </c>
+      <c r="Y8">
         <f t="shared" si="0"/>
-        <v>-3.5954886236614213E-2</v>
-      </c>
-      <c r="X8" s="8">
-        <f t="shared" si="5"/>
-        <v>5.0440518736923261</v>
-      </c>
-      <c r="Y8">
-        <f t="shared" si="1"/>
         <v>-3595.4886236614211</v>
       </c>
       <c r="Z8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>8.1305192225187053</v>
       </c>
       <c r="AA8">
@@ -11743,11 +11766,11 @@
         <v>0.72926827529815064</v>
       </c>
       <c r="AB8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>142.83414487750792</v>
       </c>
       <c r="AC8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>5.0696464122036069</v>
       </c>
       <c r="AD8">
@@ -11759,7 +11782,7 @@
         <v>10.256281104640397</v>
       </c>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>20</v>
       </c>
@@ -11779,7 +11802,7 @@
         <v>8.4898654678227725</v>
       </c>
       <c r="F9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>136.04107878372025</v>
       </c>
       <c r="G9" s="2">
@@ -11801,11 +11824,11 @@
         <v>-33.911495997140854</v>
       </c>
       <c r="L9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>7.3895502394577477</v>
       </c>
       <c r="M9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>99.568450172957938</v>
       </c>
       <c r="N9">
@@ -11822,19 +11845,19 @@
         <v>4.6E-5</v>
       </c>
       <c r="W9">
+        <f t="shared" si="3"/>
+        <v>-3.3911255261315922E-2</v>
+      </c>
+      <c r="X9" s="8">
+        <f t="shared" si="4"/>
+        <v>4.9172734252777373</v>
+      </c>
+      <c r="Y9">
         <f t="shared" si="0"/>
-        <v>-3.3911255261315922E-2</v>
-      </c>
-      <c r="X9" s="8">
-        <f t="shared" si="5"/>
-        <v>4.9172734252777373</v>
-      </c>
-      <c r="Y9">
-        <f t="shared" si="1"/>
         <v>-3391.1255261315923</v>
       </c>
       <c r="Z9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>20.436309752982879</v>
       </c>
       <c r="AA9">
@@ -11842,11 +11865,11 @@
         <v>0.70442911100721628</v>
       </c>
       <c r="AB9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>265.27163950096633</v>
       </c>
       <c r="AC9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>4.9680698223692135</v>
       </c>
       <c r="AD9">
@@ -11858,7 +11881,7 @@
         <v>15.22435092700961</v>
       </c>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>30</v>
       </c>
@@ -11878,7 +11901,7 @@
         <v>18.718350288921279</v>
       </c>
       <c r="F10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>227.12645215558851</v>
       </c>
       <c r="G10" s="2">
@@ -11900,11 +11923,11 @@
         <v>-159.15289394847926</v>
       </c>
       <c r="L10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>12.52413979513384</v>
       </c>
       <c r="M10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>181.37786811871081</v>
       </c>
       <c r="N10">
@@ -11921,19 +11944,19 @@
         <v>4.6999999999999997E-5</v>
       </c>
       <c r="W10">
+        <f t="shared" si="3"/>
+        <v>-3.0649453446594883E-2</v>
+      </c>
+      <c r="X10" s="8">
+        <f t="shared" si="4"/>
+        <v>4.9925199906818944</v>
+      </c>
+      <c r="Y10">
         <f t="shared" si="0"/>
-        <v>-3.0649453446594883E-2</v>
-      </c>
-      <c r="X10" s="8">
-        <f t="shared" si="5"/>
-        <v>4.9925199906818944</v>
-      </c>
-      <c r="Y10">
-        <f t="shared" si="1"/>
         <v>-3064.9453446594885</v>
       </c>
       <c r="Z10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>32.618018147210385</v>
       </c>
       <c r="AA10">
@@ -11941,11 +11964,11 @@
         <v>0.70074841274383914</v>
       </c>
       <c r="AB10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>407.46211529708512</v>
       </c>
       <c r="AC10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>4.910418613037475</v>
       </c>
       <c r="AD10">
@@ -11957,7 +11980,7 @@
         <v>20.134769540047085</v>
       </c>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>40</v>
       </c>
@@ -11977,7 +12000,7 @@
         <v>26.706940142196419</v>
       </c>
       <c r="F11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>315.41457294157539</v>
       </c>
       <c r="G11" s="2">
@@ -12003,7 +12026,7 @@
         <v>23.751433828608324</v>
       </c>
       <c r="M11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>264.27203817935953</v>
       </c>
       <c r="N11">
@@ -12020,19 +12043,19 @@
         <v>4.5000000000000003E-5</v>
       </c>
       <c r="W11">
+        <f t="shared" si="3"/>
+        <v>-2.5762012955374222E-2</v>
+      </c>
+      <c r="X11" s="8">
+        <f t="shared" si="4"/>
+        <v>4.7348446825001762</v>
+      </c>
+      <c r="Y11">
         <f t="shared" si="0"/>
-        <v>-2.5762012955374222E-2</v>
-      </c>
-      <c r="X11" s="8">
-        <f t="shared" si="5"/>
-        <v>4.7348446825001762</v>
-      </c>
-      <c r="Y11">
-        <f t="shared" si="1"/>
         <v>-2576.2012955374221</v>
       </c>
       <c r="Z11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>48.874404912206636</v>
       </c>
       <c r="AA11">
@@ -12040,11 +12063,11 @@
         <v>0.68806983675175393</v>
       </c>
       <c r="AB11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>529.6552766968116</v>
       </c>
       <c r="AC11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>4.8133172117323362</v>
       </c>
       <c r="AD11">
@@ -12056,7 +12079,7 @@
         <v>24.948086751779421</v>
       </c>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>50</v>
       </c>
@@ -12076,7 +12099,7 @@
         <v>36.375974446118654</v>
       </c>
       <c r="F12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>377.4346678133237</v>
       </c>
       <c r="G12" s="2">
@@ -12098,11 +12121,11 @@
         <v>-687.6969703071984</v>
       </c>
       <c r="L12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>29.102973807263588</v>
       </c>
       <c r="M12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>346.43793162427482</v>
       </c>
       <c r="N12">
@@ -12119,19 +12142,19 @@
         <v>4.6E-5</v>
       </c>
       <c r="W12">
+        <f t="shared" si="3"/>
+        <v>-2.0056347912658652E-2</v>
+      </c>
+      <c r="X12" s="8">
+        <f t="shared" si="4"/>
+        <v>4.7863687834177897</v>
+      </c>
+      <c r="Y12">
         <f t="shared" si="0"/>
-        <v>-2.0056347912658652E-2</v>
-      </c>
-      <c r="X12" s="8">
-        <f t="shared" si="5"/>
-        <v>4.7863687834177897</v>
-      </c>
-      <c r="Y12">
-        <f t="shared" si="1"/>
         <v>-2005.6347912658653</v>
       </c>
       <c r="Z12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>57.056650427155681</v>
       </c>
       <c r="AA12">
@@ -12139,11 +12162,11 @@
         <v>0.67326131849584592</v>
       </c>
       <c r="AB12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>571.88626830188207</v>
       </c>
       <c r="AC12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>4.734787287981991</v>
       </c>
       <c r="AD12">
@@ -12155,7 +12178,7 @@
         <v>29.682874039761412</v>
       </c>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>60</v>
       </c>
@@ -12175,7 +12198,7 @@
         <v>39.110959116546084</v>
       </c>
       <c r="F13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>401.86825440449763</v>
       </c>
       <c r="G13" s="2">
@@ -12201,7 +12224,7 @@
         <v>40.184612517591383</v>
       </c>
       <c r="M13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>401.91119916718122</v>
       </c>
       <c r="N13">
@@ -12218,19 +12241,19 @@
         <v>4.5000000000000003E-5</v>
       </c>
       <c r="W13">
+        <f t="shared" si="3"/>
+        <v>-1.4324287589336579E-2</v>
+      </c>
+      <c r="X13" s="8">
+        <f t="shared" si="4"/>
+        <v>4.6298419217712681</v>
+      </c>
+      <c r="Y13">
         <f t="shared" si="0"/>
-        <v>-1.4324287589336579E-2</v>
-      </c>
-      <c r="X13" s="8">
-        <f t="shared" si="5"/>
-        <v>4.6298419217712681</v>
-      </c>
-      <c r="Y13">
-        <f t="shared" si="1"/>
         <v>-1432.4287589336579</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>57.32060323322073</v>
       </c>
       <c r="AA13">
@@ -12238,11 +12261,11 @@
         <v>0.66591863130165507</v>
       </c>
       <c r="AB13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>519.3880764726523</v>
       </c>
       <c r="AC13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>4.6341089456880029</v>
       </c>
       <c r="AD13">
@@ -12254,7 +12277,7 @@
         <v>34.316982985449414</v>
       </c>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>70</v>
       </c>
@@ -12274,7 +12297,7 @@
         <v>41.262691764353441</v>
       </c>
       <c r="F14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>355.59811335189829</v>
       </c>
       <c r="G14" s="2">
@@ -12296,11 +12319,11 @@
         <v>-1491.5193686415607</v>
       </c>
       <c r="L14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>40.197627315844855</v>
       </c>
       <c r="M14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>366.85198320354584</v>
       </c>
       <c r="N14">
@@ -12317,19 +12340,19 @@
         <v>4.3999999999999999E-5</v>
       </c>
       <c r="W14">
+        <f t="shared" si="3"/>
+        <v>-9.668586383205606E-3</v>
+      </c>
+      <c r="X14" s="8">
+        <f t="shared" si="4"/>
+        <v>4.4854948790478675</v>
+      </c>
+      <c r="Y14">
         <f t="shared" si="0"/>
-        <v>-9.668586383205606E-3</v>
-      </c>
-      <c r="X14" s="8">
-        <f t="shared" si="5"/>
-        <v>4.4854948790478675</v>
-      </c>
-      <c r="Y14">
-        <f t="shared" si="1"/>
         <v>-966.85863832056054</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>46.557012061309742</v>
       </c>
       <c r="AA14">
@@ -12337,11 +12360,11 @@
         <v>0.64463245753340193</v>
       </c>
       <c r="AB14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>408.98814887661587</v>
       </c>
       <c r="AC14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>4.5394679591511551</v>
       </c>
       <c r="AD14">
@@ -12353,7 +12376,7 @@
         <v>38.856450944600567</v>
       </c>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>80</v>
       </c>
@@ -12373,7 +12396,7 @@
         <v>29.856930906026218</v>
       </c>
       <c r="F15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>253.57662827536544</v>
       </c>
       <c r="G15" s="2">
@@ -12395,11 +12418,11 @@
         <v>-1823.2470618902039</v>
       </c>
       <c r="L15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>33.172769324864319</v>
       </c>
       <c r="M15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>314.08960742805141</v>
       </c>
       <c r="N15">
@@ -12416,19 +12439,19 @@
         <v>4.5000000000000003E-5</v>
       </c>
       <c r="W15">
+        <f t="shared" si="3"/>
+        <v>-6.1445246118042619E-3</v>
+      </c>
+      <c r="X15" s="8">
+        <f t="shared" si="4"/>
+        <v>4.5554706198284114</v>
+      </c>
+      <c r="Y15">
         <f t="shared" si="0"/>
-        <v>-6.1445246118042619E-3</v>
-      </c>
-      <c r="X15" s="8">
-        <f t="shared" si="5"/>
-        <v>4.5554706198284114</v>
-      </c>
-      <c r="Y15">
-        <f t="shared" si="1"/>
         <v>-614.45246118042621</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>35.240617714013432</v>
       </c>
       <c r="AA15">
@@ -12436,11 +12459,11 @@
         <v>0.63931194950575176</v>
       </c>
       <c r="AB15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>280.60992882331675</v>
       </c>
       <c r="AC15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>4.5587749670507911</v>
       </c>
       <c r="AD15">
@@ -12452,7 +12475,7 @@
         <v>43.415225911651362</v>
       </c>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>90</v>
       </c>
@@ -12472,7 +12495,7 @@
         <v>20.858394749046873</v>
       </c>
       <c r="F16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>152.15825683147114</v>
       </c>
       <c r="G16" s="2">
@@ -12494,11 +12517,11 @@
         <v>-2119.6985834976635</v>
       </c>
       <c r="L16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>29.645152160745965</v>
       </c>
       <c r="M16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>249.47766059694595</v>
       </c>
       <c r="N16">
@@ -12515,19 +12538,19 @@
         <v>4.6E-5</v>
       </c>
       <c r="W16">
+        <f t="shared" si="3"/>
+        <v>-4.0563878067392707E-3</v>
+      </c>
+      <c r="X16" s="8">
+        <f t="shared" si="4"/>
+        <v>4.6373944575193793</v>
+      </c>
+      <c r="Y16">
         <f t="shared" si="0"/>
-        <v>-4.0563878067392707E-3</v>
-      </c>
-      <c r="X16" s="8">
-        <f t="shared" si="5"/>
-        <v>4.6373944575193793</v>
-      </c>
-      <c r="Y16">
-        <f t="shared" si="1"/>
         <v>-405.63878067392704</v>
       </c>
       <c r="Z16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>20.881368050649918</v>
       </c>
       <c r="AA16">
@@ -12535,11 +12558,11 @@
         <v>0.65005953514083081</v>
       </c>
       <c r="AB16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>157.93178101382384</v>
       </c>
       <c r="AC16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>4.5895563424163957</v>
       </c>
       <c r="AD16">
@@ -12551,7 +12574,7 @@
         <v>48.004782254067756</v>
       </c>
     </row>
-    <row r="17" spans="1:34">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>100</v>
       </c>
@@ -12593,11 +12616,11 @@
         <v>-2322.2023830840958</v>
       </c>
       <c r="L17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>20.250379958643226</v>
       </c>
       <c r="M17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>101.25189979321613</v>
       </c>
       <c r="N17">
@@ -12614,19 +12637,19 @@
         <v>4.5000000000000003E-5</v>
       </c>
       <c r="W17">
+        <f t="shared" si="3"/>
+        <v>-2.9858889915277856E-3</v>
+      </c>
+      <c r="X17" s="8">
+        <f t="shared" si="4"/>
+        <v>4.5269131208225639</v>
+      </c>
+      <c r="Y17">
         <f t="shared" si="0"/>
-        <v>-2.9858889915277856E-3</v>
-      </c>
-      <c r="X17" s="8">
-        <f t="shared" si="5"/>
-        <v>4.5269131208225639</v>
-      </c>
-      <c r="Y17">
-        <f t="shared" si="1"/>
         <v>-298.58889915277854</v>
       </c>
       <c r="Z17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>10.704988152114851</v>
       </c>
       <c r="AA17">
@@ -12634,11 +12657,11 @@
         <v>0.64806149212946562</v>
       </c>
       <c r="AB17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>27.567267850308937</v>
       </c>
       <c r="AC17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>3.5877148982223552</v>
       </c>
       <c r="AD17">
@@ -12650,7 +12673,7 @@
         <v>51.592497152290107</v>
       </c>
     </row>
-    <row r="18" spans="1:34" ht="14.65" thickBot="1">
+    <row r="18" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="T18" s="28">
         <v>105</v>
       </c>
@@ -12661,19 +12684,19 @@
         <v>4.5000000000000003E-5</v>
       </c>
       <c r="W18" s="30">
+        <f t="shared" si="3"/>
+        <v>-3.0019849409282217E-3</v>
+      </c>
+      <c r="X18" s="29">
+        <f t="shared" si="4"/>
+        <v>4.5270584180794886</v>
+      </c>
+      <c r="Y18" s="30">
         <f t="shared" si="0"/>
-        <v>-3.0019849409282217E-3</v>
-      </c>
-      <c r="X18" s="29">
-        <f t="shared" si="5"/>
-        <v>4.5270584180794886</v>
-      </c>
-      <c r="Y18" s="30">
-        <f t="shared" si="1"/>
         <v>-300.19849409282216</v>
       </c>
       <c r="Z18" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.32191898800872421</v>
       </c>
       <c r="AA18" s="30">
@@ -12697,37 +12720,37 @@
         <v>54.793559488616125</v>
       </c>
     </row>
-    <row r="20" spans="1:34" ht="14.65" thickBot="1"/>
-    <row r="21" spans="1:34" ht="28.5">
-      <c r="A21" s="48" t="s">
+    <row r="20" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:34" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="49"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="6"/>
-      <c r="J21" s="48" t="s">
+      <c r="J21" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="K21" s="49"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="49"/>
-      <c r="N21" s="49"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="50"/>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
       <c r="R21" s="6"/>
-      <c r="T21" s="50" t="s">
+      <c r="T21" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="U21" s="51"/>
-      <c r="V21" s="51"/>
-      <c r="W21" s="51"/>
-      <c r="X21" s="51"/>
+      <c r="U21" s="52"/>
+      <c r="V21" s="52"/>
+      <c r="W21" s="52"/>
+      <c r="X21" s="52"/>
       <c r="Y21" s="24"/>
       <c r="Z21" s="24"/>
       <c r="AA21" s="24"/>
@@ -12739,7 +12762,7 @@
       <c r="AG21" s="32"/>
       <c r="AH21" s="32"/>
     </row>
-    <row r="22" spans="1:34">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
@@ -12797,7 +12820,7 @@
       <c r="T22" s="26"/>
       <c r="AE22" s="27"/>
     </row>
-    <row r="23" spans="1:34">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>0.14285714285714199</v>
       </c>
@@ -12865,7 +12888,7 @@
       <c r="T23" s="26"/>
       <c r="AE23" s="27"/>
     </row>
-    <row r="24" spans="1:34">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>10.285714285714199</v>
       </c>
@@ -12967,7 +12990,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:34">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>20.428571428571399</v>
       </c>
@@ -13066,7 +13089,7 @@
       </c>
       <c r="AE25" s="27"/>
     </row>
-    <row r="26" spans="1:34">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>30.714285714285701</v>
       </c>
@@ -13170,7 +13193,7 @@
       </c>
       <c r="AE26" s="27"/>
     </row>
-    <row r="27" spans="1:34">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>40.857142857142797</v>
       </c>
@@ -13281,7 +13304,7 @@
         <v>5.0273289162865797</v>
       </c>
     </row>
-    <row r="28" spans="1:34">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>50.428571428571402</v>
       </c>
@@ -13392,7 +13415,7 @@
         <v>10.038408468611976</v>
       </c>
     </row>
-    <row r="29" spans="1:34">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>60.571428571428498</v>
       </c>
@@ -13503,7 +13526,7 @@
         <v>14.913976117615197</v>
       </c>
     </row>
-    <row r="30" spans="1:34">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>70.428571428571402</v>
       </c>
@@ -13614,7 +13637,7 @@
         <v>19.694135640406735</v>
       </c>
     </row>
-    <row r="31" spans="1:34">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>80.428571428571402</v>
       </c>
@@ -13725,7 +13748,7 @@
         <v>24.477320255294085</v>
       </c>
     </row>
-    <row r="32" spans="1:34">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>90.142857142857096</v>
       </c>
@@ -13836,7 +13859,7 @@
         <v>29.262045678150127</v>
       </c>
     </row>
-    <row r="33" spans="1:34">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>100.142857142857</v>
       </c>
@@ -13947,7 +13970,7 @@
         <v>33.899914323664056</v>
       </c>
     </row>
-    <row r="34" spans="1:34">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="F34">
         <v>50.428571428571402</v>
@@ -14024,7 +14047,7 @@
         <v>38.421329609798718</v>
       </c>
     </row>
-    <row r="35" spans="1:34">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="F35">
         <v>53.857142857142797</v>
@@ -14101,7 +14124,7 @@
         <v>42.942323774857194</v>
       </c>
     </row>
-    <row r="36" spans="1:34">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="F36">
         <v>56.142857142857103</v>
@@ -14178,7 +14201,7 @@
         <v>47.473133093663868</v>
       </c>
     </row>
-    <row r="37" spans="1:34">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="F37">
         <v>72.285714285714207</v>
@@ -14255,7 +14278,7 @@
         <v>51.099500900938892</v>
       </c>
     </row>
-    <row r="38" spans="1:34" ht="14.65" thickBot="1">
+    <row r="38" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="F38">
         <v>76.142857142857096</v>
@@ -14333,7 +14356,7 @@
         <v>54.349424291828953</v>
       </c>
     </row>
-    <row r="39" spans="1:34">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="F39">
         <v>81.428571428571402</v>
@@ -14365,7 +14388,7 @@
         <v>2856.7810526315752</v>
       </c>
     </row>
-    <row r="40" spans="1:34" ht="28.5">
+    <row r="40" spans="1:34" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A40" s="1"/>
       <c r="F40">
         <v>88.142857142857096</v>
@@ -14383,26 +14406,26 @@
       </c>
       <c r="J40" s="1"/>
       <c r="R40" s="2"/>
-      <c r="T40" s="48" t="s">
+      <c r="T40" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="U40" s="49"/>
-      <c r="V40" s="49"/>
-      <c r="W40" s="49"/>
-      <c r="X40" s="49"/>
+      <c r="U40" s="50"/>
+      <c r="V40" s="50"/>
+      <c r="W40" s="50"/>
+      <c r="X40" s="50"/>
       <c r="Y40" s="5"/>
       <c r="Z40" s="6"/>
-      <c r="AB40" s="48" t="s">
+      <c r="AB40" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="AC40" s="49"/>
-      <c r="AD40" s="49"/>
-      <c r="AE40" s="49"/>
-      <c r="AF40" s="49"/>
+      <c r="AC40" s="50"/>
+      <c r="AD40" s="50"/>
+      <c r="AE40" s="50"/>
+      <c r="AF40" s="50"/>
       <c r="AG40" s="5"/>
       <c r="AH40" s="6"/>
     </row>
-    <row r="41" spans="1:34">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="F41">
         <v>98.428571428571402</v>
@@ -14425,7 +14448,7 @@
       <c r="AB41" s="1"/>
       <c r="AH41" s="2"/>
     </row>
-    <row r="42" spans="1:34">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -14459,7 +14482,7 @@
       <c r="AB42" s="1"/>
       <c r="AH42" s="2"/>
     </row>
-    <row r="43" spans="1:34">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.25">
       <c r="T43" s="1" t="s">
         <v>3</v>
       </c>
@@ -14503,7 +14526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:34">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.25">
       <c r="T44" s="1">
         <v>-20</v>
       </c>
@@ -14550,7 +14573,7 @@
       </c>
       <c r="AH44" s="2"/>
     </row>
-    <row r="45" spans="1:34">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.25">
       <c r="T45" s="1">
         <v>-10</v>
       </c>
@@ -14598,7 +14621,7 @@
       </c>
       <c r="AH45" s="2"/>
     </row>
-    <row r="46" spans="1:34">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.25">
       <c r="T46" s="1">
         <v>0</v>
       </c>
@@ -14652,7 +14675,7 @@
         <v>173.64372251132431</v>
       </c>
     </row>
-    <row r="47" spans="1:34">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.25">
       <c r="T47" s="1">
         <v>10</v>
       </c>
@@ -14706,7 +14729,7 @@
         <v>407.90251503308286</v>
       </c>
     </row>
-    <row r="48" spans="1:34">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.25">
       <c r="T48" s="1">
         <v>20</v>
       </c>
@@ -14760,7 +14783,7 @@
         <v>760.83947308657935</v>
       </c>
     </row>
-    <row r="49" spans="20:34">
+    <row r="49" spans="20:34" x14ac:dyDescent="0.25">
       <c r="T49" s="1">
         <v>30</v>
       </c>
@@ -14814,7 +14837,7 @@
         <v>1236.2236555511472</v>
       </c>
     </row>
-    <row r="50" spans="20:34">
+    <row r="50" spans="20:34" x14ac:dyDescent="0.25">
       <c r="T50" s="1">
         <v>40</v>
       </c>
@@ -14868,7 +14891,7 @@
         <v>1784.023158835932</v>
       </c>
     </row>
-    <row r="51" spans="20:34">
+    <row r="51" spans="20:34" x14ac:dyDescent="0.25">
       <c r="T51" s="1">
         <v>50</v>
       </c>
@@ -14922,7 +14945,7 @@
         <v>2327.0530879851167</v>
       </c>
     </row>
-    <row r="52" spans="20:34">
+    <row r="52" spans="20:34" x14ac:dyDescent="0.25">
       <c r="T52" s="1">
         <v>60</v>
       </c>
@@ -14976,7 +14999,7 @@
         <v>2785.0254040158216</v>
       </c>
     </row>
-    <row r="53" spans="20:34">
+    <row r="53" spans="20:34" x14ac:dyDescent="0.25">
       <c r="T53" s="1">
         <v>70</v>
       </c>
@@ -15030,7 +15053,7 @@
         <v>3122.9075717257065</v>
       </c>
     </row>
-    <row r="54" spans="20:34">
+    <row r="54" spans="20:34" x14ac:dyDescent="0.25">
       <c r="T54" s="1">
         <v>80</v>
       </c>
@@ -15084,7 +15107,7 @@
         <v>3339.7873384462846</v>
       </c>
     </row>
-    <row r="55" spans="20:34">
+    <row r="55" spans="20:34" x14ac:dyDescent="0.25">
       <c r="T55" s="1">
         <v>90</v>
       </c>
@@ -15138,7 +15161,7 @@
         <v>3469.3977628558255</v>
       </c>
     </row>
-    <row r="56" spans="20:34">
+    <row r="56" spans="20:34" x14ac:dyDescent="0.25">
       <c r="T56" s="1">
         <v>100</v>
       </c>
@@ -15192,7 +15215,7 @@
         <v>3495.0967379467706</v>
       </c>
     </row>
-    <row r="57" spans="20:34">
+    <row r="57" spans="20:34" x14ac:dyDescent="0.25">
       <c r="T57" s="3">
         <v>105</v>
       </c>
@@ -15267,75 +15290,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A0E277-164D-40AC-8934-6E7AB0E9B78A}">
   <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="topRight" activeCell="N23" sqref="N23"/>
+      <selection pane="topRight" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="18.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.1328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.1328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="53"/>
-      <c r="H1" s="55" t="s">
+      <c r="G1" s="56"/>
+      <c r="H1" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="M1" s="57" t="s">
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="M1" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
     </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
       <c r="F2" s="18" t="s">
         <v>25</v>
       </c>
@@ -15373,7 +15396,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>32</v>
       </c>
@@ -15423,11 +15446,11 @@
         <f>P3/N3^2</f>
         <v>5.2209776578745846</v>
       </c>
-      <c r="S3" s="56"/>
-      <c r="T3" s="56"/>
-      <c r="U3" s="56"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="58"/>
+      <c r="U3" s="58"/>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>36</v>
       </c>
@@ -15476,11 +15499,11 @@
         <f t="shared" ref="R4:R14" si="2">P4/N4^2</f>
         <v>5.4716504320242159</v>
       </c>
-      <c r="S4" s="56"/>
-      <c r="T4" s="56"/>
-      <c r="U4" s="56"/>
+      <c r="S4" s="58"/>
+      <c r="T4" s="58"/>
+      <c r="U4" s="58"/>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>38</v>
       </c>
@@ -15529,11 +15552,11 @@
         <f t="shared" si="2"/>
         <v>5.2211869240932307</v>
       </c>
-      <c r="S5" s="56"/>
-      <c r="T5" s="56"/>
-      <c r="U5" s="56"/>
+      <c r="S5" s="58"/>
+      <c r="T5" s="58"/>
+      <c r="U5" s="58"/>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>40</v>
       </c>
@@ -15582,7 +15605,7 @@
         <v>5.2197850806303423</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>42</v>
       </c>
@@ -15632,7 +15655,7 @@
         <v>5.2206428580925941</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>44</v>
       </c>
@@ -15680,7 +15703,7 @@
         <v>5.5241804399646828</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>46</v>
       </c>
@@ -15728,7 +15751,7 @@
         <v>4.4512457342260809</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>44</v>
       </c>
@@ -15776,7 +15799,7 @@
         <v>5.4686443952612604</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>44</v>
       </c>
@@ -15824,7 +15847,7 @@
         <v>5.5596163140471271</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="M12" t="s">
         <v>52</v>
       </c>
@@ -15849,7 +15872,7 @@
         <v>4.2462509186260418</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="M13" t="s">
         <v>53</v>
       </c>
@@ -15874,7 +15897,7 @@
         <v>5.3532710417581892</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="M14" t="s">
         <v>54</v>
       </c>
@@ -15899,48 +15922,48 @@
         <v>5.3404035488093591</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M17" s="8"/>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
-      <c r="A24" s="53" t="s">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="53" t="s">
+      <c r="B24" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="53" t="s">
+      <c r="C24" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="53" t="s">
+      <c r="D24" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="53" t="s">
+      <c r="E24" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="53" t="s">
+      <c r="F24" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="G24" s="53"/>
-      <c r="H24" s="55" t="s">
+      <c r="G24" s="56"/>
+      <c r="H24" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="I24" s="55"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="55"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="54"/>
       <c r="N24" s="8"/>
     </row>
-    <row r="25" spans="1:14">
-      <c r="A25" s="54"/>
-      <c r="B25" s="54"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="57"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
       <c r="F25" s="18" t="s">
         <v>25</v>
       </c>
@@ -15966,7 +15989,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>32</v>
       </c>
@@ -16013,7 +16036,7 @@
         <v>113.23848291901987</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>36</v>
       </c>
@@ -16062,7 +16085,7 @@
         <v>100.45037434596571</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>38</v>
       </c>
@@ -16111,7 +16134,7 @@
         <v>91.573165076947419</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>40</v>
       </c>
@@ -16160,7 +16183,7 @@
         <v>71.791289229976712</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>42</v>
       </c>
@@ -16209,7 +16232,7 @@
         <v>68.212607735624033</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>44</v>
       </c>
@@ -16246,7 +16269,7 @@
         <v>7.9583946693193894</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>46</v>
       </c>
@@ -16283,7 +16306,7 @@
         <v>23.783317867529405</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
         <v>44</v>
       </c>
@@ -16320,7 +16343,7 @@
         <v>7.4904492223462142</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
         <v>44</v>
       </c>
@@ -16357,17 +16380,17 @@
         <v>9.2086121231703402</v>
       </c>
     </row>
-    <row r="39" spans="1:18">
-      <c r="A39" s="57" t="s">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="57"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="57"/>
-      <c r="F39" s="57"/>
+      <c r="B39" s="55"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="55"/>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>61</v>
       </c>
@@ -16421,7 +16444,7 @@
         <v>9.9999999999999998E+23</v>
       </c>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>77</v>
       </c>
@@ -16478,7 +16501,7 @@
         <v>2.54</v>
       </c>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -16536,7 +16559,7 @@
         <v>6.0650947308232492</v>
       </c>
     </row>
-    <row r="43" spans="1:18">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>38</v>
       </c>
@@ -16601,7 +16624,7 @@
         <v>0.26600000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:18">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>40</v>
       </c>
@@ -16665,7 +16688,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -16730,7 +16753,7 @@
         <v>0.67564000000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:18">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -16787,7 +16810,7 @@
         <v>35.56</v>
       </c>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -16844,7 +16867,7 @@
         <v>50.996730261790482</v>
       </c>
     </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>44</v>
       </c>
@@ -16901,7 +16924,7 @@
         <v>6.0221408E+23</v>
       </c>
     </row>
-    <row r="49" spans="1:18">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>44</v>
       </c>
@@ -16959,6 +16982,17 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="M1:R1"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="H24:K24"/>
     <mergeCell ref="A39:F39"/>
     <mergeCell ref="A24:A25"/>
@@ -16967,17 +17001,6 @@
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="E24:E25"/>
     <mergeCell ref="F24:G24"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="M1:R1"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -16992,17 +17015,17 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>86</v>
       </c>
@@ -17019,7 +17042,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -17038,7 +17061,7 @@
         <v>26.99999999999994</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -17057,7 +17080,7 @@
         <v>15.52296296296297</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -17080,10 +17103,10 @@
         <v>214.75512375340509</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" s="13"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -17099,20 +17122,20 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="A9" sqref="A9:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1328125" customWidth="1"/>
-    <col min="5" max="5" width="19.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>96</v>
       </c>
@@ -17132,7 +17155,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>102</v>
       </c>
@@ -17152,7 +17175,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>103</v>
       </c>
@@ -17172,7 +17195,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>104</v>
       </c>
@@ -17192,7 +17215,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -17212,7 +17235,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -17232,7 +17255,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -17256,7 +17279,7 @@
         <v>7.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>107</v>
       </c>
@@ -17276,7 +17299,7 @@
         <v>2879.8</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>146</v>
       </c>
@@ -17301,7 +17324,7 @@
         <v>1.0296519158733199</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75">
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>114</v>
       </c>
@@ -17321,7 +17344,7 @@
         <v>1.02627</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>147</v>
       </c>
@@ -17346,7 +17369,7 @@
         <v>1.5900000000000002E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>129</v>
       </c>
@@ -17371,7 +17394,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>108</v>
       </c>
@@ -17396,7 +17419,7 @@
         <v>2559.7552301051428</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>116</v>
       </c>
@@ -17421,7 +17444,7 @@
         <v>5.0321386894330216</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>115</v>
       </c>
@@ -17446,7 +17469,7 @@
         <v>-320.04476989485738</v>
       </c>
     </row>
-    <row r="20" spans="6:6">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F20" s="22"/>
     </row>
   </sheetData>
@@ -17464,24 +17487,24 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>120</v>
       </c>
@@ -17496,7 +17519,7 @@
       </c>
       <c r="E1" s="33"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -17510,7 +17533,7 @@
         <v>-4.3</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>119</v>
       </c>
@@ -17526,7 +17549,7 @@
         <v>7.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>107</v>
       </c>
@@ -17547,7 +17570,7 @@
       <c r="M4" s="8"/>
       <c r="O4" s="8"/>
     </row>
-    <row r="5" spans="1:15" ht="15.75">
+    <row r="5" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -17566,7 +17589,7 @@
       <c r="M5" s="8"/>
       <c r="O5" s="8"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>117</v>
       </c>
@@ -17587,7 +17610,7 @@
       <c r="M6" s="8"/>
       <c r="O6" s="8"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>108</v>
       </c>
@@ -17605,7 +17628,7 @@
       </c>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>116</v>
       </c>
@@ -17622,7 +17645,7 @@
         <v>5.3170540466255174</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -17638,7 +17661,7 @@
         <v>-49.483069181355262</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -17654,7 +17677,7 @@
         <v>-16.373069181355262</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -17670,13 +17693,13 @@
         <v>6.7247956311301511</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F13">
         <f>2.3/100*10^5*0.0077</f>
         <v>17.71</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>167</v>
       </c>
@@ -17699,14 +17722,14 @@
       <selection activeCell="C19" sqref="C19:D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>130</v>
       </c>
@@ -17717,7 +17740,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>133</v>
       </c>
@@ -17728,7 +17751,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>134</v>
       </c>
@@ -17739,7 +17762,7 @@
         <v>0.53200000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -17750,7 +17773,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>136</v>
       </c>
@@ -17761,7 +17784,7 @@
         <v>309.02300000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>137</v>
       </c>
@@ -17772,7 +17795,7 @@
         <v>30.4</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>138</v>
       </c>
@@ -17783,7 +17806,7 @@
         <v>93.14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>145</v>
       </c>
@@ -17794,7 +17817,7 @@
         <v>5.96E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>139</v>
       </c>
@@ -17805,7 +17828,7 @@
         <v>9.84</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>140</v>
       </c>
@@ -17816,7 +17839,7 @@
         <v>88.52</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>141</v>
       </c>
@@ -17827,7 +17850,7 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>142</v>
       </c>
@@ -17838,7 +17861,7 @@
         <v>1.67</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>143</v>
       </c>
@@ -17862,15 +17885,15 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.53125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>96</v>
       </c>
@@ -17890,7 +17913,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -17910,7 +17933,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -17934,7 +17957,7 @@
         <v>7.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>107</v>
       </c>
@@ -17957,7 +17980,7 @@
         <v>2879.8</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>146</v>
       </c>
@@ -17982,7 +18005,7 @@
         <v>1.0296519158733199</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75">
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>114</v>
       </c>
@@ -18004,7 +18027,7 @@
         <v>1.02627</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>129</v>
       </c>
@@ -18029,7 +18052,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>108</v>
       </c>
@@ -18054,7 +18077,7 @@
         <v>2559.7552301051428</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>116</v>
       </c>
@@ -18079,7 +18102,7 @@
         <v>5.0321386894330216</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>115</v>
       </c>
@@ -18111,19 +18134,21 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21ED06BD-0914-45E0-871D-AD003873F521}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="33"/>
       <c r="B1" s="33"/>
       <c r="C1" s="33"/>
@@ -18131,7 +18156,7 @@
       <c r="E1" s="33"/>
       <c r="F1" s="33"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>151</v>
       </c>
@@ -18148,7 +18173,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>150</v>
       </c>
@@ -18165,7 +18190,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>156</v>
       </c>
@@ -18182,7 +18207,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>162</v>
       </c>
@@ -18198,8 +18223,15 @@
       <c r="E5">
         <v>1.71</v>
       </c>
+      <c r="H5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I5">
+        <f>C9*6-'Critical Configuration'!D13</f>
+        <v>2434.539172911343</v>
+      </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>106</v>
       </c>
@@ -18215,8 +18247,15 @@
       <c r="E6" s="37">
         <v>7.7000000000000002E-3</v>
       </c>
+      <c r="H6" t="s">
+        <v>184</v>
+      </c>
+      <c r="I6">
+        <f>I5/6</f>
+        <v>405.75652881855717</v>
+      </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>163</v>
       </c>
@@ -18237,7 +18276,7 @@
         <v>1316.7</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>155</v>
       </c>
@@ -18253,18 +18292,18 @@
         <f>D4/100*D6*10^5</f>
         <v>315.7</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="48">
         <f>E4/100*E6*10^5</f>
         <v>219.45</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>157</v>
       </c>
       <c r="B9" s="37">
-        <f>B21/6-D21-C21</f>
-        <v>473.84651883711035</v>
+        <f>(6*C9-B21-E21)/6</f>
+        <v>396.09546556857441</v>
       </c>
       <c r="C9" s="37">
         <f>E21-D21</f>
@@ -18279,13 +18318,13 @@
         <v>200.93018857352263</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>158</v>
       </c>
       <c r="B10" s="37">
-        <f>SQRT((1/6)^2*B20^2+D20^2)</f>
-        <v>8.4334156781223584</v>
+        <f>SQRT((6*C10)^2*B20^2+D20^2)/6</f>
+        <v>40.3162808304536</v>
       </c>
       <c r="C10" s="37">
         <f>SQRT(E20^2+D20^2)</f>
@@ -18301,13 +18340,13 @@
       </c>
       <c r="F10" s="23"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>164</v>
       </c>
       <c r="B11" s="38">
         <f>B9-B8</f>
-        <v>21.856518837110343</v>
+        <v>-55.894534431425598</v>
       </c>
       <c r="C11" s="38">
         <f>C9-C8</f>
@@ -18322,13 +18361,13 @@
         <v>-18.519811426477361</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>165</v>
       </c>
       <c r="B12">
         <f>B9*6-B7</f>
-        <v>132.67911302266202</v>
+        <v>-333.82720658855351</v>
       </c>
       <c r="C12">
         <f t="shared" ref="C12:E12" si="1">C9*6-C7</f>
@@ -18342,21 +18381,28 @@
         <f t="shared" si="1"/>
         <v>-111.11886855886428</v>
       </c>
+      <c r="H12" t="s">
+        <v>183</v>
+      </c>
+      <c r="I12">
+        <f>C7+B21-E21</f>
+        <v>1826.9576790684921</v>
+      </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>166</v>
       </c>
       <c r="B13">
-        <f>SQRT(36*B10^2)</f>
-        <v>50.60049406873415</v>
+        <f>6*B10</f>
+        <v>241.89768498272161</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:E13" si="2">SQRT(36*C10^2)</f>
+        <f>SQRT(36*C10^2)</f>
         <v>53.722620933830108</v>
       </c>
       <c r="D13">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D13:E13" si="2">SQRT(36*D10^2)</f>
         <v>62.81687671318911</v>
       </c>
       <c r="E13">
@@ -18364,14 +18410,21 @@
         <v>71.701882820467134</v>
       </c>
       <c r="F13" s="36"/>
+      <c r="H13" t="s">
+        <v>184</v>
+      </c>
+      <c r="I13">
+        <f>I12/6</f>
+        <v>304.49294651141537</v>
+      </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F14" s="34"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F15" s="36"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>96</v>
       </c>
@@ -18382,7 +18435,7 @@
         <v>110</v>
       </c>
       <c r="D17" t="s">
-        <v>152</v>
+        <v>185</v>
       </c>
       <c r="E17" t="s">
         <v>159</v>
@@ -18394,13 +18447,12 @@
         <v>161</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75">
+    <row r="18" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>114</v>
       </c>
       <c r="B18">
-        <f>0.956965</f>
-        <v>0.95696499999999995</v>
+        <v>0.99760300000000002</v>
       </c>
       <c r="C18">
         <v>0.990927</v>
@@ -18419,7 +18471,7 @@
         <v>0.99893299999999996</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>147</v>
       </c>
@@ -18444,7 +18496,7 @@
         <v>8.5000000000000006E-5</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>129</v>
       </c>
@@ -18473,16 +18525,16 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>108</v>
       </c>
       <c r="B21">
-        <f t="shared" ref="B21:G21" si="4">(1-1/B18)*10^5</f>
-        <v>-4497.0296719315738</v>
+        <f>(1-1/B18)*10^5</f>
+        <v>-240.27594143161136</v>
       </c>
       <c r="C21">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="C21:G21" si="4">(1-1/C18)*10^5</f>
         <v>-915.6073050789804</v>
       </c>
       <c r="D21">
@@ -18502,16 +18554,16 @@
         <v>-106.81397050653629</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>116</v>
       </c>
       <c r="B22">
-        <f t="shared" ref="B22:G22" si="5">(B20/B18^2)</f>
-        <v>4.9138331446154471</v>
+        <f>(B20/B18^2)</f>
+        <v>4.5216508143664589</v>
       </c>
       <c r="C22">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="C22:G22" si="5">(C20/C18^2)</f>
         <v>8.8600450240450304</v>
       </c>
       <c r="D22">
@@ -18531,13 +18583,65 @@
         <v>8.5181680728267626</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="36"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>186</v>
+      </c>
+      <c r="B25">
+        <f>B9*6</f>
+        <v>2376.5727934114466</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25:E25" si="6">C9*6</f>
+        <v>2194.2632314797315</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="6"/>
+        <v>1732.9606818238476</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="6"/>
+        <v>1205.5811314411358</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>115</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="B26">
+        <f>B10*6</f>
+        <v>241.89768498272161</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ref="C26:E26" si="7">C10*6</f>
+        <v>53.7226209338301</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="7"/>
+        <v>62.816876713189103</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="7"/>
+        <v>71.701882820467134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="35"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="35"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18553,19 +18657,19 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A1" s="58" t="s">
         <v>173</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
     </row>
-    <row r="2" spans="1:101">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>174</v>
       </c>
@@ -18870,7 +18974,7 @@
         <v>0.22126297517171509</v>
       </c>
     </row>
-    <row r="3" spans="1:101">
+    <row r="3" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>175</v>
       </c>
@@ -19175,7 +19279,7 @@
         <v>18.009399999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:101">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>178</v>
       </c>
@@ -19480,7 +19584,7 @@
         <v>9.4699999999999993E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:101">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>179</v>
       </c>
@@ -19885,7 +19989,7 @@
         <v>2.8409999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:101">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>177</v>
       </c>
@@ -19914,7 +20018,7 @@
         <v>0.29187749667110502</v>
       </c>
     </row>
-    <row r="7" spans="1:101">
+    <row r="7" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>176</v>
       </c>
@@ -19953,15 +20057,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ABEDCDC6898E9D48B17B2D917023A0E9" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c9b35f98bcdb4a0d7929321150581d5e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="02f07221-7782-4248-899f-09bd431cf93f" xmlns:ns3="e1ecaa1f-5549-4843-8e0b-36d11b9c4a00" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="53fe39de12092328c3276185799bfa71" ns2:_="" ns3:_="">
     <xsd:import namespace="02f07221-7782-4248-899f-09bd431cf93f"/>
@@ -20198,6 +20293,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -20217,14 +20321,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC7DCD2E-E082-4B2B-AAD1-C045E4862869}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4FEB34B-0950-495E-8A7D-7F2024A133DD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20239,6 +20335,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC7DCD2E-E082-4B2B-AAD1-C045E4862869}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>